<commit_message>
fixed all errors, notified Trevor
</commit_message>
<xml_diff>
--- a/AMOS 2018 SEASON OUTPUT DRAFT 20180103.xlsx
+++ b/AMOS 2018 SEASON OUTPUT DRAFT 20180103.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Documents\SportsAnalytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73536805-F80F-409C-92AB-B1752B891348}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4981D850-0860-40FD-919D-F366DE8D05F4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1008,7 +1008,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="17"/>
@@ -1033,6 +1033,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1396,7 +1399,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>10</c:v>
@@ -2163,7 +2166,7 @@
                   <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.5625</c:v>
+                  <c:v>0.625</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.66666666666666663</c:v>
@@ -2964,7 +2967,7 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>38</c:v>
@@ -4465,7 +4468,7 @@
                   <c:v>0.48837209302325579</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.68235294117647061</c:v>
+                  <c:v>0.69411764705882351</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.79166666666666663</c:v>
@@ -6043,7 +6046,7 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>58</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>85</c:v>
@@ -10855,10 +10858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD259"/>
+  <dimension ref="A1:AG259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="W35" sqref="W35"/>
+    <sheetView tabSelected="1" topLeftCell="P10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z38" sqref="Z38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10893,7 +10896,7 @@
     <col min="30" max="30" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10973,7 +10976,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11064,8 +11067,12 @@
         <f>SUM(V2/W2)</f>
         <v>0.5</v>
       </c>
+      <c r="AG2" t="str">
+        <f>IF(OR(OR(AND(I2&gt;0.5, M2=1, N2=1), AND(I2&lt;0.5, M2=0, N2=1), AND(I2&gt;0.5, M2=0, N2=0), AND(I2&lt;0.5, M2=1, N2=0)), OR(AND(J2&gt;0.5, M2=1, O2=1), AND(J2&lt;0.5, M2=0, O2=1), AND(J2&gt;0.5, M2=0, O2=0), AND(J2&lt;0.5, M2=1, O2=0)), OR(AND(K2&gt;0.5, M2=1, P2=1), AND(K2&lt;0.5, M2=0, P2=1), AND(K2&gt;0.5, M2=0, P2=0), AND(K2&lt;0.5, M2=1, P2=0)), OR(AND(L2&gt;0.5, M2=1, Q2=1), AND(L2&lt;0.5, M2=0, Q2=1), AND(L2&gt;0.5, M2=0, Q2=0), AND(L2&lt;0.5, M2=1, Q2=0))), "", "XXX")</f>
+        <v/>
+      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -11156,8 +11163,12 @@
         <f t="shared" ref="AA3:AA18" si="5">SUM(V3/W3)</f>
         <v>0.625</v>
       </c>
+      <c r="AG3" t="str">
+        <f t="shared" ref="AG3:AG66" si="6">IF(OR(OR(AND(I3&gt;0.5, M3=1, N3=1), AND(I3&lt;0.5, M3=0, N3=1), AND(I3&gt;0.5, M3=0, N3=0), AND(I3&lt;0.5, M3=1, N3=0)), OR(AND(J3&gt;0.5, M3=1, O3=1), AND(J3&lt;0.5, M3=0, O3=1), AND(J3&gt;0.5, M3=0, O3=0), AND(J3&lt;0.5, M3=1, O3=0)), OR(AND(K3&gt;0.5, M3=1, P3=1), AND(K3&lt;0.5, M3=0, P3=1), AND(K3&gt;0.5, M3=0, P3=0), AND(K3&lt;0.5, M3=1, P3=0)), OR(AND(L3&gt;0.5, M3=1, Q3=1), AND(L3&lt;0.5, M3=0, Q3=1), AND(L3&gt;0.5, M3=0, Q3=0), AND(L3&lt;0.5, M3=1, Q3=0))), "", "XXX")</f>
+        <v/>
+      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -11217,15 +11228,15 @@
         <v>10</v>
       </c>
       <c r="T4">
-        <f t="shared" ref="T4:V4" si="6">SUM(O34:O49)</f>
+        <f t="shared" ref="T4:V4" si="7">SUM(O34:O49)</f>
         <v>8</v>
       </c>
       <c r="U4">
-        <f t="shared" si="6"/>
-        <v>9</v>
+        <f t="shared" si="7"/>
+        <v>10</v>
       </c>
       <c r="V4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="W4">
@@ -11242,14 +11253,18 @@
       </c>
       <c r="Z4">
         <f t="shared" si="4"/>
-        <v>0.5625</v>
+        <v>0.625</v>
       </c>
       <c r="AA4">
         <f t="shared" si="5"/>
         <v>0.6875</v>
       </c>
+      <c r="AG4" t="str">
+        <f t="shared" si="6"/>
+        <v>XXX</v>
+      </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -11309,15 +11324,15 @@
         <v>8</v>
       </c>
       <c r="T5">
-        <f t="shared" ref="T5:V5" si="7">SUM(O50:O64)</f>
+        <f t="shared" ref="T5:V5" si="8">SUM(O50:O64)</f>
         <v>11</v>
       </c>
       <c r="U5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="V5">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="W5">
@@ -11340,8 +11355,12 @@
         <f t="shared" si="5"/>
         <v>0.73333333333333328</v>
       </c>
+      <c r="AG5" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
@@ -11401,15 +11420,15 @@
         <v>7</v>
       </c>
       <c r="T6">
-        <f t="shared" ref="T6:V6" si="8">SUM(O65:O79)</f>
+        <f t="shared" ref="T6:V6" si="9">SUM(O65:O79)</f>
         <v>10</v>
       </c>
       <c r="U6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="V6">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="W6">
@@ -11432,8 +11451,12 @@
         <f t="shared" si="5"/>
         <v>0.66666666666666663</v>
       </c>
+      <c r="AG6" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -11493,15 +11516,15 @@
         <v>11</v>
       </c>
       <c r="T7">
-        <f t="shared" ref="T7:V7" si="9">SUM(O80:O94)</f>
+        <f t="shared" ref="T7:V7" si="10">SUM(O80:O94)</f>
         <v>11</v>
       </c>
       <c r="U7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
       <c r="V7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11</v>
       </c>
       <c r="W7">
@@ -11524,8 +11547,12 @@
         <f t="shared" si="5"/>
         <v>0.73333333333333328</v>
       </c>
+      <c r="AG7" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -11585,15 +11612,15 @@
         <v>8</v>
       </c>
       <c r="T8">
-        <f t="shared" ref="T8:V8" si="10">SUM(O95:O108)</f>
+        <f t="shared" ref="T8:V8" si="11">SUM(O95:O108)</f>
         <v>8</v>
       </c>
       <c r="U8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="V8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>8</v>
       </c>
       <c r="W8">
@@ -11616,8 +11643,12 @@
         <f t="shared" si="5"/>
         <v>0.5714285714285714</v>
       </c>
+      <c r="AG8" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -11677,15 +11708,15 @@
         <v>8</v>
       </c>
       <c r="T9">
-        <f t="shared" ref="T9:V9" si="11">SUM(O109:O122)</f>
+        <f t="shared" ref="T9:V9" si="12">SUM(O109:O122)</f>
         <v>11</v>
       </c>
       <c r="U9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="V9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>9</v>
       </c>
       <c r="W9">
@@ -11708,8 +11739,12 @@
         <f t="shared" si="5"/>
         <v>0.6428571428571429</v>
       </c>
+      <c r="AG9" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -11769,15 +11804,15 @@
         <v>6</v>
       </c>
       <c r="T10">
-        <f t="shared" ref="T10:V10" si="12">SUM(O123:O135)</f>
+        <f t="shared" ref="T10:V10" si="13">SUM(O123:O135)</f>
         <v>8</v>
       </c>
       <c r="U10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="V10">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
       <c r="W10">
@@ -11800,8 +11835,12 @@
         <f t="shared" si="5"/>
         <v>0.61538461538461542</v>
       </c>
+      <c r="AG10" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -11861,15 +11900,15 @@
         <v>10</v>
       </c>
       <c r="T11">
-        <f t="shared" ref="T11:V11" si="13">SUM(O136:O149)</f>
+        <f t="shared" ref="T11:V11" si="14">SUM(O136:O149)</f>
         <v>8</v>
       </c>
       <c r="U11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="V11">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="W11">
@@ -11892,8 +11931,12 @@
         <f t="shared" si="5"/>
         <v>0.5714285714285714</v>
       </c>
+      <c r="AG11" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -11953,15 +11996,15 @@
         <v>6</v>
       </c>
       <c r="T12">
-        <f t="shared" ref="T12:V12" si="14">SUM(O150:O162)</f>
+        <f t="shared" ref="T12:V12" si="15">SUM(O150:O162)</f>
         <v>7</v>
       </c>
       <c r="U12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="V12">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>9</v>
       </c>
       <c r="W12">
@@ -11984,8 +12027,12 @@
         <f t="shared" si="5"/>
         <v>0.69230769230769229</v>
       </c>
+      <c r="AG12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -12045,15 +12092,15 @@
         <v>12</v>
       </c>
       <c r="T13">
-        <f t="shared" ref="T13:V13" si="15">SUM(O163:O177)</f>
+        <f t="shared" ref="T13:V13" si="16">SUM(O163:O177)</f>
         <v>12</v>
       </c>
       <c r="U13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="V13">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>12</v>
       </c>
       <c r="W13">
@@ -12076,8 +12123,12 @@
         <f t="shared" si="5"/>
         <v>0.8</v>
       </c>
+      <c r="AG13" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -12137,15 +12188,15 @@
         <v>10</v>
       </c>
       <c r="T14">
-        <f t="shared" ref="T14:V14" si="16">SUM(O178:O193)</f>
+        <f t="shared" ref="T14:V14" si="17">SUM(O178:O193)</f>
         <v>8</v>
       </c>
       <c r="U14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>10</v>
       </c>
       <c r="V14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9</v>
       </c>
       <c r="W14">
@@ -12168,8 +12219,12 @@
         <f t="shared" si="5"/>
         <v>0.5625</v>
       </c>
+      <c r="AG14" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -12229,15 +12284,15 @@
         <v>7</v>
       </c>
       <c r="T15">
-        <f t="shared" ref="T15:V15" si="17">SUM(O194:O209)</f>
+        <f t="shared" ref="T15:V15" si="18">SUM(O194:O209)</f>
         <v>7</v>
       </c>
       <c r="U15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="V15">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="W15">
@@ -12260,8 +12315,12 @@
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
+      <c r="AG15" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -12321,15 +12380,15 @@
         <v>7</v>
       </c>
       <c r="T16">
-        <f t="shared" ref="T16:V16" si="18">SUM(O210:O225)</f>
+        <f t="shared" ref="T16:V16" si="19">SUM(O210:O225)</f>
         <v>9</v>
       </c>
       <c r="U16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="V16">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>10</v>
       </c>
       <c r="W16">
@@ -12352,8 +12411,12 @@
         <f t="shared" si="5"/>
         <v>0.625</v>
       </c>
+      <c r="AG16" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -12413,15 +12476,15 @@
         <v>11</v>
       </c>
       <c r="T17">
-        <f t="shared" ref="T17:V17" si="19">SUM(O226:O241)</f>
+        <f t="shared" ref="T17:V17" si="20">SUM(O226:O241)</f>
         <v>11</v>
       </c>
       <c r="U17">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9</v>
       </c>
       <c r="V17">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>11</v>
       </c>
       <c r="W17">
@@ -12444,8 +12507,12 @@
         <f t="shared" si="5"/>
         <v>0.6875</v>
       </c>
+      <c r="AG17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -12505,15 +12572,15 @@
         <v>12</v>
       </c>
       <c r="T18">
-        <f t="shared" ref="T18:V18" si="20">SUM(O242:O257)</f>
+        <f t="shared" ref="T18:V18" si="21">SUM(O242:O257)</f>
         <v>12</v>
       </c>
       <c r="U18">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
       <c r="V18">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>12</v>
       </c>
       <c r="W18">
@@ -12536,8 +12603,12 @@
         <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
+      <c r="AG18" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="19" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -12597,15 +12668,15 @@
         <v>8.882352941176471</v>
       </c>
       <c r="T19" s="2">
-        <f t="shared" ref="T19:V19" si="21">AVERAGE(T2:T18)</f>
+        <f t="shared" ref="T19:V19" si="22">AVERAGE(T2:T18)</f>
         <v>9.3529411764705888</v>
       </c>
       <c r="U19" s="2">
-        <f t="shared" si="21"/>
-        <v>9.6470588235294112</v>
+        <f t="shared" si="22"/>
+        <v>9.7058823529411757</v>
       </c>
       <c r="V19" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>9.7058823529411757</v>
       </c>
       <c r="X19" s="5">
@@ -12613,19 +12684,23 @@
         <v>0.58829724197371247</v>
       </c>
       <c r="Y19" s="5">
-        <f t="shared" ref="Y19:AA19" si="22">AVERAGE(Y2:Y18)</f>
+        <f t="shared" ref="Y19:AA19" si="23">AVERAGE(Y2:Y18)</f>
         <v>0.62225005386770083</v>
       </c>
       <c r="Z19" s="5">
-        <f t="shared" si="22"/>
-        <v>0.64256625727213956</v>
+        <f t="shared" si="23"/>
+        <v>0.64624272786037484</v>
       </c>
       <c r="AA19" s="5">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>0.64495528980823102</v>
       </c>
+      <c r="AG19" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="20" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -12682,19 +12757,23 @@
         <v>151</v>
       </c>
       <c r="T20">
-        <f t="shared" ref="T20:V20" si="23">SUM(T2:T18)</f>
+        <f t="shared" ref="T20:V20" si="24">SUM(T2:T18)</f>
         <v>159</v>
       </c>
       <c r="U20">
-        <f t="shared" si="23"/>
-        <v>164</v>
+        <f t="shared" si="24"/>
+        <v>165</v>
       </c>
       <c r="V20">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>165</v>
       </c>
+      <c r="AG20" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -12746,8 +12825,12 @@
       <c r="Q21">
         <v>0</v>
       </c>
+      <c r="AG21" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -12799,8 +12882,12 @@
       <c r="Q22">
         <v>1</v>
       </c>
+      <c r="AG22" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -12852,8 +12939,12 @@
       <c r="Q23">
         <v>0</v>
       </c>
+      <c r="AG23" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -12944,8 +13035,12 @@
       <c r="AD24" s="10" t="s">
         <v>148</v>
       </c>
+      <c r="AG24" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -12997,7 +13092,7 @@
       <c r="Q25">
         <v>0</v>
       </c>
-      <c r="R25" s="8" t="s">
+      <c r="R25" s="14" t="s">
         <v>130</v>
       </c>
       <c r="S25">
@@ -13021,7 +13116,7 @@
         <v>2</v>
       </c>
       <c r="X25">
-        <f>SUM(V25/W25)</f>
+        <f t="shared" ref="X25:X32" si="25">SUM(V25/W25)</f>
         <v>1</v>
       </c>
       <c r="Y25">
@@ -13044,11 +13139,15 @@
         <v>3</v>
       </c>
       <c r="AD25">
-        <f>SUM(AB25/AC25)</f>
-        <v>1</v>
+        <f t="shared" ref="AD25:AD32" si="26">SUM(AB25/AC25)</f>
+        <v>1</v>
+      </c>
+      <c r="AG25" t="str">
+        <f t="shared" si="6"/>
+        <v/>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -13100,7 +13199,7 @@
       <c r="Q26">
         <v>1</v>
       </c>
-      <c r="R26" s="8" t="s">
+      <c r="R26" s="14" t="s">
         <v>129</v>
       </c>
       <c r="S26">
@@ -13124,7 +13223,7 @@
         <v>13</v>
       </c>
       <c r="X26">
-        <f>SUM(V26/W26)</f>
+        <f t="shared" si="25"/>
         <v>0.53846153846153844</v>
       </c>
       <c r="Y26">
@@ -13136,7 +13235,7 @@
         <v>21</v>
       </c>
       <c r="AA26">
-        <f>SUM(Y26/Z26)</f>
+        <f t="shared" ref="AA26:AA32" si="27">SUM(Y26/Z26)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AB26">
@@ -13148,11 +13247,15 @@
         <v>12</v>
       </c>
       <c r="AD26">
-        <f>SUM(AB26/AC26)</f>
+        <f t="shared" si="26"/>
         <v>0.75</v>
       </c>
+      <c r="AG26" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -13204,7 +13307,7 @@
       <c r="Q27">
         <v>0</v>
       </c>
-      <c r="R27" s="8" t="s">
+      <c r="R27" s="14" t="s">
         <v>131</v>
       </c>
       <c r="S27">
@@ -13216,7 +13319,7 @@
         <v>47</v>
       </c>
       <c r="U27">
-        <f t="shared" ref="U27:U32" si="24">SUM(S27/T27)</f>
+        <f t="shared" ref="U27:U32" si="28">SUM(S27/T27)</f>
         <v>0.55319148936170215</v>
       </c>
       <c r="V27">
@@ -13228,7 +13331,7 @@
         <v>27</v>
       </c>
       <c r="X27">
-        <f>SUM(V27/W27)</f>
+        <f t="shared" si="25"/>
         <v>0.59259259259259256</v>
       </c>
       <c r="Y27">
@@ -13240,7 +13343,7 @@
         <v>22</v>
       </c>
       <c r="AA27">
-        <f>SUM(Y27/Z27)</f>
+        <f t="shared" si="27"/>
         <v>0.59090909090909094</v>
       </c>
       <c r="AB27">
@@ -13252,11 +13355,15 @@
         <v>23</v>
       </c>
       <c r="AD27">
-        <f>SUM(AB27/AC27)</f>
+        <f t="shared" si="26"/>
         <v>0.52173913043478259</v>
       </c>
+      <c r="AG27" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -13308,7 +13415,7 @@
       <c r="Q28">
         <v>1</v>
       </c>
-      <c r="R28" s="8" t="s">
+      <c r="R28" s="14" t="s">
         <v>132</v>
       </c>
       <c r="S28">
@@ -13320,7 +13427,7 @@
         <v>41</v>
       </c>
       <c r="U28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0.41463414634146339</v>
       </c>
       <c r="V28">
@@ -13332,7 +13439,7 @@
         <v>28</v>
       </c>
       <c r="X28">
-        <f>SUM(V28/W28)</f>
+        <f t="shared" si="25"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="Y28">
@@ -13344,7 +13451,7 @@
         <v>33</v>
       </c>
       <c r="AA28">
-        <f>SUM(Y28/Z28)</f>
+        <f t="shared" si="27"/>
         <v>0.48484848484848486</v>
       </c>
       <c r="AB28">
@@ -13356,11 +13463,15 @@
         <v>35</v>
       </c>
       <c r="AD28">
-        <f>SUM(AB28/AC28)</f>
+        <f t="shared" si="26"/>
         <v>0.51428571428571423</v>
       </c>
+      <c r="AG28" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -13412,7 +13523,7 @@
       <c r="Q29">
         <v>1</v>
       </c>
-      <c r="R29" s="8" t="s">
+      <c r="R29" s="14" t="s">
         <v>133</v>
       </c>
       <c r="S29">
@@ -13424,7 +13535,7 @@
         <v>25</v>
       </c>
       <c r="U29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="V29">
@@ -13436,7 +13547,7 @@
         <v>50</v>
       </c>
       <c r="X29">
-        <f>SUM(V29/W29)</f>
+        <f t="shared" si="25"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="Y29">
@@ -13448,7 +13559,7 @@
         <v>43</v>
       </c>
       <c r="AA29">
-        <f>SUM(Y29/Z29)</f>
+        <f t="shared" si="27"/>
         <v>0.48837209302325579</v>
       </c>
       <c r="AB29">
@@ -13460,11 +13571,15 @@
         <v>50</v>
       </c>
       <c r="AD29">
-        <f>SUM(AB29/AC29)</f>
+        <f t="shared" si="26"/>
         <v>0.46</v>
       </c>
+      <c r="AG29" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -13528,7 +13643,7 @@
         <v>44</v>
       </c>
       <c r="U30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0.63636363636363635</v>
       </c>
       <c r="V30">
@@ -13540,20 +13655,20 @@
         <v>70</v>
       </c>
       <c r="X30">
-        <f>SUM(V30/W30)</f>
+        <f t="shared" si="25"/>
         <v>0.6</v>
       </c>
       <c r="Y30">
         <f>COUNTIFS(K2:K257,"&gt;=0.6", K2:K257,"&lt;0.7", P2:P257,"1")</f>
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Z30">
         <f>COUNTIFS(K2:K257,"&gt;=0.6",K2:K257,"&lt;0.7")</f>
         <v>85</v>
       </c>
       <c r="AA30">
-        <f>SUM(Y30/Z30)</f>
-        <v>0.68235294117647061</v>
+        <f t="shared" si="27"/>
+        <v>0.69411764705882351</v>
       </c>
       <c r="AB30">
         <f>COUNTIFS(L2:L257,"&gt;=0.6", L2:L257,"&lt;0.7", Q2:Q257,"1")</f>
@@ -13564,11 +13679,15 @@
         <v>53</v>
       </c>
       <c r="AD30">
-        <f>SUM(AB30/AC30)</f>
+        <f t="shared" si="26"/>
         <v>0.67924528301886788</v>
       </c>
+      <c r="AG30" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -13620,7 +13739,7 @@
       <c r="Q31">
         <v>1</v>
       </c>
-      <c r="R31" s="8" t="s">
+      <c r="R31" s="14" t="s">
         <v>135</v>
       </c>
       <c r="S31">
@@ -13632,7 +13751,7 @@
         <v>47</v>
       </c>
       <c r="U31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0.78723404255319152</v>
       </c>
       <c r="V31">
@@ -13644,7 +13763,7 @@
         <v>41</v>
       </c>
       <c r="X31">
-        <f>SUM(V31/W31)</f>
+        <f t="shared" si="25"/>
         <v>0.70731707317073167</v>
       </c>
       <c r="Y31">
@@ -13656,7 +13775,7 @@
         <v>48</v>
       </c>
       <c r="AA31">
-        <f>SUM(Y31/Z31)</f>
+        <f t="shared" si="27"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="AB31">
@@ -13668,11 +13787,15 @@
         <v>53</v>
       </c>
       <c r="AD31">
-        <f>SUM(AB31/AC31)</f>
+        <f t="shared" si="26"/>
         <v>0.79245283018867929</v>
       </c>
+      <c r="AG31" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>
@@ -13724,11 +13847,11 @@
       <c r="Q32">
         <v>1</v>
       </c>
-      <c r="R32" s="8" t="s">
+      <c r="R32" s="14" t="s">
         <v>136</v>
       </c>
       <c r="S32">
-        <f>SUM(COUNTIFS(I2:I257,"&gt;=0.8",M2:M257,1)-COUNTIFS(I2:I257,"1",M2:M257,1))</f>
+        <f>COUNTIFS(I2:I257,"&gt;=0.8", I2:I257,"&lt;1", N2:N257,"1")</f>
         <v>22</v>
       </c>
       <c r="T32">
@@ -13736,7 +13859,7 @@
         <v>36</v>
       </c>
       <c r="U32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0.61111111111111116</v>
       </c>
       <c r="V32">
@@ -13748,7 +13871,7 @@
         <v>25</v>
       </c>
       <c r="X32">
-        <f>SUM(V32/W32)</f>
+        <f t="shared" si="25"/>
         <v>0.92</v>
       </c>
       <c r="Y32">
@@ -13760,7 +13883,7 @@
         <v>4</v>
       </c>
       <c r="AA32">
-        <f>SUM(Y32/Z32)</f>
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
       <c r="AB32">
@@ -13772,11 +13895,15 @@
         <v>27</v>
       </c>
       <c r="AD32">
-        <f>SUM(AB32/AC32)</f>
+        <f t="shared" si="26"/>
         <v>0.81481481481481477</v>
       </c>
+      <c r="AG32" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="33" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -13857,7 +13984,7 @@
       </c>
       <c r="Y33" s="2">
         <f>SUM(Y25:Y32)</f>
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="Z33" s="2">
         <f>SUM(Z25:Z32)</f>
@@ -13865,7 +13992,7 @@
       </c>
       <c r="AA33" s="2">
         <f>AVERAGE(AA26:AA32)</f>
-        <v>0.67211656332723357</v>
+        <v>0.67379723559614113</v>
       </c>
       <c r="AB33" s="2">
         <f>SUM(AB25:AB32)</f>
@@ -13879,8 +14006,12 @@
         <f>AVERAGE(AD25:AD32)</f>
         <v>0.69156722159285733</v>
       </c>
+      <c r="AG33" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="34" spans="1:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -13933,8 +14064,12 @@
         <v>1</v>
       </c>
       <c r="R34" s="9"/>
+      <c r="AG34" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -13986,8 +14121,12 @@
       <c r="Q35">
         <v>0</v>
       </c>
+      <c r="AG35" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -14039,8 +14178,12 @@
       <c r="Q36">
         <v>1</v>
       </c>
+      <c r="AG36" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3</v>
       </c>
@@ -14092,8 +14235,12 @@
       <c r="Q37">
         <v>1</v>
       </c>
+      <c r="AG37" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -14145,8 +14292,12 @@
       <c r="Q38">
         <v>0</v>
       </c>
+      <c r="AG38" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -14198,8 +14349,12 @@
       <c r="Q39">
         <v>0</v>
       </c>
+      <c r="AG39" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -14251,8 +14406,12 @@
       <c r="Q40">
         <v>1</v>
       </c>
+      <c r="AG40" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>3</v>
       </c>
@@ -14304,8 +14463,12 @@
       <c r="Q41">
         <v>1</v>
       </c>
+      <c r="AG41" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -14357,8 +14520,12 @@
       <c r="Q42">
         <v>0</v>
       </c>
+      <c r="AG42" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -14410,8 +14577,12 @@
       <c r="Q43">
         <v>1</v>
       </c>
+      <c r="AG43" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
@@ -14463,8 +14634,12 @@
       <c r="Q44">
         <v>1</v>
       </c>
+      <c r="AG44" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
@@ -14516,8 +14691,12 @@
       <c r="Q45">
         <v>1</v>
       </c>
+      <c r="AG45" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -14569,8 +14748,12 @@
       <c r="Q46">
         <v>1</v>
       </c>
+      <c r="AG46" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>3</v>
       </c>
@@ -14622,8 +14805,12 @@
       <c r="Q47">
         <v>1</v>
       </c>
+      <c r="AG47" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -14670,13 +14857,17 @@
         <v>0</v>
       </c>
       <c r="P48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q48">
         <v>0</v>
       </c>
+      <c r="AG48" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>3</v>
       </c>
@@ -14728,8 +14919,12 @@
       <c r="Q49">
         <v>1</v>
       </c>
+      <c r="AG49" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>4</v>
       </c>
@@ -14781,8 +14976,12 @@
       <c r="Q50">
         <v>1</v>
       </c>
+      <c r="AG50" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -14834,8 +15033,12 @@
       <c r="Q51">
         <v>0</v>
       </c>
+      <c r="AG51" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>4</v>
       </c>
@@ -14887,8 +15090,12 @@
       <c r="Q52">
         <v>1</v>
       </c>
+      <c r="AG52" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>4</v>
       </c>
@@ -14940,8 +15147,12 @@
       <c r="Q53">
         <v>1</v>
       </c>
+      <c r="AG53" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>4</v>
       </c>
@@ -14993,8 +15204,12 @@
       <c r="Q54">
         <v>1</v>
       </c>
+      <c r="AG54" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>4</v>
       </c>
@@ -15046,8 +15261,12 @@
       <c r="Q55">
         <v>0</v>
       </c>
+      <c r="AG55" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>4</v>
       </c>
@@ -15099,8 +15318,12 @@
       <c r="Q56">
         <v>1</v>
       </c>
+      <c r="AG56" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>4</v>
       </c>
@@ -15152,8 +15375,12 @@
       <c r="Q57">
         <v>1</v>
       </c>
+      <c r="AG57" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>4</v>
       </c>
@@ -15205,8 +15432,12 @@
       <c r="Q58">
         <v>0</v>
       </c>
+      <c r="AG58" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>4</v>
       </c>
@@ -15258,8 +15489,12 @@
       <c r="Q59">
         <v>1</v>
       </c>
+      <c r="AG59" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>4</v>
       </c>
@@ -15311,8 +15546,12 @@
       <c r="Q60">
         <v>1</v>
       </c>
+      <c r="AG60" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>4</v>
       </c>
@@ -15364,8 +15603,12 @@
       <c r="Q61">
         <v>1</v>
       </c>
+      <c r="AG61" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>4</v>
       </c>
@@ -15417,8 +15660,12 @@
       <c r="Q62">
         <v>1</v>
       </c>
+      <c r="AG62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>4</v>
       </c>
@@ -15470,8 +15717,12 @@
       <c r="Q63">
         <v>0</v>
       </c>
+      <c r="AG63" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>4</v>
       </c>
@@ -15523,8 +15774,12 @@
       <c r="Q64">
         <v>1</v>
       </c>
+      <c r="AG64" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>5</v>
       </c>
@@ -15576,8 +15831,12 @@
       <c r="Q65">
         <v>1</v>
       </c>
+      <c r="AG65" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>5</v>
       </c>
@@ -15629,8 +15888,12 @@
       <c r="Q66">
         <v>0</v>
       </c>
+      <c r="AG66" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>5</v>
       </c>
@@ -15682,8 +15945,12 @@
       <c r="Q67">
         <v>1</v>
       </c>
+      <c r="AG67" t="str">
+        <f t="shared" ref="AG67:AG130" si="29">IF(OR(OR(AND(I67&gt;0.5, M67=1, N67=1), AND(I67&lt;0.5, M67=0, N67=1), AND(I67&gt;0.5, M67=0, N67=0), AND(I67&lt;0.5, M67=1, N67=0)), OR(AND(J67&gt;0.5, M67=1, O67=1), AND(J67&lt;0.5, M67=0, O67=1), AND(J67&gt;0.5, M67=0, O67=0), AND(J67&lt;0.5, M67=1, O67=0)), OR(AND(K67&gt;0.5, M67=1, P67=1), AND(K67&lt;0.5, M67=0, P67=1), AND(K67&gt;0.5, M67=0, P67=0), AND(K67&lt;0.5, M67=1, P67=0)), OR(AND(L67&gt;0.5, M67=1, Q67=1), AND(L67&lt;0.5, M67=0, Q67=1), AND(L67&gt;0.5, M67=0, Q67=0), AND(L67&lt;0.5, M67=1, Q67=0))), "", "XXX")</f>
+        <v/>
+      </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>5</v>
       </c>
@@ -15735,8 +16002,12 @@
       <c r="Q68">
         <v>1</v>
       </c>
+      <c r="AG68" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>5</v>
       </c>
@@ -15788,8 +16059,12 @@
       <c r="Q69">
         <v>0</v>
       </c>
+      <c r="AG69" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>5</v>
       </c>
@@ -15841,8 +16116,12 @@
       <c r="Q70">
         <v>0</v>
       </c>
+      <c r="AG70" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>5</v>
       </c>
@@ -15894,8 +16173,12 @@
       <c r="Q71">
         <v>1</v>
       </c>
+      <c r="AG71" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>5</v>
       </c>
@@ -15947,8 +16230,12 @@
       <c r="Q72">
         <v>1</v>
       </c>
+      <c r="AG72" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>5</v>
       </c>
@@ -16000,8 +16287,12 @@
       <c r="Q73">
         <v>1</v>
       </c>
+      <c r="AG73" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>5</v>
       </c>
@@ -16053,8 +16344,12 @@
       <c r="Q74">
         <v>1</v>
       </c>
+      <c r="AG74" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>5</v>
       </c>
@@ -16106,8 +16401,12 @@
       <c r="Q75">
         <v>0</v>
       </c>
+      <c r="AG75" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>5</v>
       </c>
@@ -16159,8 +16458,12 @@
       <c r="Q76">
         <v>0</v>
       </c>
+      <c r="AG76" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>5</v>
       </c>
@@ -16212,8 +16515,12 @@
       <c r="Q77">
         <v>1</v>
       </c>
+      <c r="AG77" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>5</v>
       </c>
@@ -16265,8 +16572,12 @@
       <c r="Q78">
         <v>1</v>
       </c>
+      <c r="AG78" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>5</v>
       </c>
@@ -16318,8 +16629,12 @@
       <c r="Q79">
         <v>1</v>
       </c>
+      <c r="AG79" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>6</v>
       </c>
@@ -16371,8 +16686,12 @@
       <c r="Q80">
         <v>0</v>
       </c>
+      <c r="AG80" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>6</v>
       </c>
@@ -16424,8 +16743,12 @@
       <c r="Q81">
         <v>1</v>
       </c>
+      <c r="AG81" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>6</v>
       </c>
@@ -16477,8 +16800,12 @@
       <c r="Q82">
         <v>0</v>
       </c>
+      <c r="AG82" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>6</v>
       </c>
@@ -16530,8 +16857,12 @@
       <c r="Q83">
         <v>1</v>
       </c>
+      <c r="AG83" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>6</v>
       </c>
@@ -16583,8 +16914,12 @@
       <c r="Q84">
         <v>1</v>
       </c>
+      <c r="AG84" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>6</v>
       </c>
@@ -16636,8 +16971,12 @@
       <c r="Q85">
         <v>0</v>
       </c>
+      <c r="AG85" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>6</v>
       </c>
@@ -16689,8 +17028,12 @@
       <c r="Q86">
         <v>1</v>
       </c>
+      <c r="AG86" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>6</v>
       </c>
@@ -16742,8 +17085,12 @@
       <c r="Q87">
         <v>0</v>
       </c>
+      <c r="AG87" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>6</v>
       </c>
@@ -16795,8 +17142,12 @@
       <c r="Q88">
         <v>1</v>
       </c>
+      <c r="AG88" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>6</v>
       </c>
@@ -16848,8 +17199,12 @@
       <c r="Q89">
         <v>1</v>
       </c>
+      <c r="AG89" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>6</v>
       </c>
@@ -16901,8 +17256,12 @@
       <c r="Q90">
         <v>1</v>
       </c>
+      <c r="AG90" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>6</v>
       </c>
@@ -16954,8 +17313,12 @@
       <c r="Q91">
         <v>1</v>
       </c>
+      <c r="AG91" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>6</v>
       </c>
@@ -17007,8 +17370,12 @@
       <c r="Q92">
         <v>1</v>
       </c>
+      <c r="AG92" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>6</v>
       </c>
@@ -17060,8 +17427,12 @@
       <c r="Q93">
         <v>1</v>
       </c>
+      <c r="AG93" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>6</v>
       </c>
@@ -17113,8 +17484,12 @@
       <c r="Q94">
         <v>1</v>
       </c>
+      <c r="AG94" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>7</v>
       </c>
@@ -17166,8 +17541,12 @@
       <c r="Q95">
         <v>1</v>
       </c>
+      <c r="AG95" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>7</v>
       </c>
@@ -17219,8 +17598,12 @@
       <c r="Q96">
         <v>0</v>
       </c>
+      <c r="AG96" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>7</v>
       </c>
@@ -17272,8 +17655,12 @@
       <c r="Q97">
         <v>1</v>
       </c>
+      <c r="AG97" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>7</v>
       </c>
@@ -17325,8 +17712,12 @@
       <c r="Q98">
         <v>0</v>
       </c>
+      <c r="AG98" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>7</v>
       </c>
@@ -17378,8 +17769,12 @@
       <c r="Q99">
         <v>1</v>
       </c>
+      <c r="AG99" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>7</v>
       </c>
@@ -17431,8 +17826,12 @@
       <c r="Q100">
         <v>0</v>
       </c>
+      <c r="AG100" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>7</v>
       </c>
@@ -17484,8 +17883,12 @@
       <c r="Q101">
         <v>1</v>
       </c>
+      <c r="AG101" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>7</v>
       </c>
@@ -17537,8 +17940,12 @@
       <c r="Q102">
         <v>0</v>
       </c>
+      <c r="AG102" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>7</v>
       </c>
@@ -17590,8 +17997,12 @@
       <c r="Q103">
         <v>1</v>
       </c>
+      <c r="AG103" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>7</v>
       </c>
@@ -17643,8 +18054,12 @@
       <c r="Q104">
         <v>0</v>
       </c>
+      <c r="AG104" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>7</v>
       </c>
@@ -17696,8 +18111,12 @@
       <c r="Q105">
         <v>0</v>
       </c>
+      <c r="AG105" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>7</v>
       </c>
@@ -17749,8 +18168,12 @@
       <c r="Q106">
         <v>1</v>
       </c>
+      <c r="AG106" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>7</v>
       </c>
@@ -17802,8 +18225,12 @@
       <c r="Q107">
         <v>1</v>
       </c>
+      <c r="AG107" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>7</v>
       </c>
@@ -17855,8 +18282,12 @@
       <c r="Q108">
         <v>1</v>
       </c>
+      <c r="AG108" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>8</v>
       </c>
@@ -17908,8 +18339,12 @@
       <c r="Q109">
         <v>1</v>
       </c>
+      <c r="AG109" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>8</v>
       </c>
@@ -17961,8 +18396,12 @@
       <c r="Q110">
         <v>0</v>
       </c>
+      <c r="AG110" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>8</v>
       </c>
@@ -18014,8 +18453,12 @@
       <c r="Q111">
         <v>1</v>
       </c>
+      <c r="AG111" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>8</v>
       </c>
@@ -18067,8 +18510,12 @@
       <c r="Q112">
         <v>1</v>
       </c>
+      <c r="AG112" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>8</v>
       </c>
@@ -18120,8 +18567,12 @@
       <c r="Q113">
         <v>1</v>
       </c>
+      <c r="AG113" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>8</v>
       </c>
@@ -18173,8 +18624,12 @@
       <c r="Q114">
         <v>1</v>
       </c>
+      <c r="AG114" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>8</v>
       </c>
@@ -18226,8 +18681,12 @@
       <c r="Q115">
         <v>0</v>
       </c>
+      <c r="AG115" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>8</v>
       </c>
@@ -18279,8 +18738,12 @@
       <c r="Q116">
         <v>1</v>
       </c>
+      <c r="AG116" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>8</v>
       </c>
@@ -18332,8 +18795,12 @@
       <c r="Q117">
         <v>0</v>
       </c>
+      <c r="AG117" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>8</v>
       </c>
@@ -18385,8 +18852,12 @@
       <c r="Q118">
         <v>0</v>
       </c>
+      <c r="AG118" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>8</v>
       </c>
@@ -18438,8 +18909,12 @@
       <c r="Q119">
         <v>1</v>
       </c>
+      <c r="AG119" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>8</v>
       </c>
@@ -18491,8 +18966,12 @@
       <c r="Q120">
         <v>0</v>
       </c>
+      <c r="AG120" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>8</v>
       </c>
@@ -18544,8 +19023,12 @@
       <c r="Q121">
         <v>1</v>
       </c>
+      <c r="AG121" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>8</v>
       </c>
@@ -18597,8 +19080,12 @@
       <c r="Q122">
         <v>1</v>
       </c>
+      <c r="AG122" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>9</v>
       </c>
@@ -18650,8 +19137,12 @@
       <c r="Q123">
         <v>1</v>
       </c>
+      <c r="AG123" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>9</v>
       </c>
@@ -18703,8 +19194,12 @@
       <c r="Q124">
         <v>0</v>
       </c>
+      <c r="AG124" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>9</v>
       </c>
@@ -18756,8 +19251,12 @@
       <c r="Q125">
         <v>1</v>
       </c>
+      <c r="AG125" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>9</v>
       </c>
@@ -18809,8 +19308,12 @@
       <c r="Q126">
         <v>1</v>
       </c>
+      <c r="AG126" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>9</v>
       </c>
@@ -18862,8 +19365,12 @@
       <c r="Q127">
         <v>1</v>
       </c>
+      <c r="AG127" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>9</v>
       </c>
@@ -18915,8 +19422,12 @@
       <c r="Q128">
         <v>1</v>
       </c>
+      <c r="AG128" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="129" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>9</v>
       </c>
@@ -18968,8 +19479,12 @@
       <c r="Q129">
         <v>1</v>
       </c>
+      <c r="AG129" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>9</v>
       </c>
@@ -19021,8 +19536,12 @@
       <c r="Q130">
         <v>1</v>
       </c>
+      <c r="AG130" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>9</v>
       </c>
@@ -19074,8 +19593,12 @@
       <c r="Q131">
         <v>0</v>
       </c>
+      <c r="AG131" t="str">
+        <f t="shared" ref="AG131:AG194" si="30">IF(OR(OR(AND(I131&gt;0.5, M131=1, N131=1), AND(I131&lt;0.5, M131=0, N131=1), AND(I131&gt;0.5, M131=0, N131=0), AND(I131&lt;0.5, M131=1, N131=0)), OR(AND(J131&gt;0.5, M131=1, O131=1), AND(J131&lt;0.5, M131=0, O131=1), AND(J131&gt;0.5, M131=0, O131=0), AND(J131&lt;0.5, M131=1, O131=0)), OR(AND(K131&gt;0.5, M131=1, P131=1), AND(K131&lt;0.5, M131=0, P131=1), AND(K131&gt;0.5, M131=0, P131=0), AND(K131&lt;0.5, M131=1, P131=0)), OR(AND(L131&gt;0.5, M131=1, Q131=1), AND(L131&lt;0.5, M131=0, Q131=1), AND(L131&gt;0.5, M131=0, Q131=0), AND(L131&lt;0.5, M131=1, Q131=0))), "", "XXX")</f>
+        <v/>
+      </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>9</v>
       </c>
@@ -19127,8 +19650,12 @@
       <c r="Q132">
         <v>0</v>
       </c>
+      <c r="AG132" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>9</v>
       </c>
@@ -19180,8 +19707,12 @@
       <c r="Q133">
         <v>0</v>
       </c>
+      <c r="AG133" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>9</v>
       </c>
@@ -19233,8 +19764,12 @@
       <c r="Q134">
         <v>1</v>
       </c>
+      <c r="AG134" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="135" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>9</v>
       </c>
@@ -19286,8 +19821,12 @@
       <c r="Q135">
         <v>0</v>
       </c>
+      <c r="AG135" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>10</v>
       </c>
@@ -19339,8 +19878,12 @@
       <c r="Q136">
         <v>1</v>
       </c>
+      <c r="AG136" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>10</v>
       </c>
@@ -19392,8 +19935,12 @@
       <c r="Q137">
         <v>1</v>
       </c>
+      <c r="AG137" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>10</v>
       </c>
@@ -19445,8 +19992,12 @@
       <c r="Q138">
         <v>1</v>
       </c>
+      <c r="AG138" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>10</v>
       </c>
@@ -19498,8 +20049,12 @@
       <c r="Q139">
         <v>0</v>
       </c>
+      <c r="AG139" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>10</v>
       </c>
@@ -19551,8 +20106,12 @@
       <c r="Q140">
         <v>1</v>
       </c>
+      <c r="AG140" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="141" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>10</v>
       </c>
@@ -19604,8 +20163,12 @@
       <c r="Q141">
         <v>1</v>
       </c>
+      <c r="AG141" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>10</v>
       </c>
@@ -19657,8 +20220,12 @@
       <c r="Q142">
         <v>1</v>
       </c>
+      <c r="AG142" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>10</v>
       </c>
@@ -19710,8 +20277,12 @@
       <c r="Q143">
         <v>0</v>
       </c>
+      <c r="AG143" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>10</v>
       </c>
@@ -19763,8 +20334,12 @@
       <c r="Q144">
         <v>0</v>
       </c>
+      <c r="AG144" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>10</v>
       </c>
@@ -19816,8 +20391,12 @@
       <c r="Q145">
         <v>0</v>
       </c>
+      <c r="AG145" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>10</v>
       </c>
@@ -19869,8 +20448,12 @@
       <c r="Q146">
         <v>1</v>
       </c>
+      <c r="AG146" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>10</v>
       </c>
@@ -19922,8 +20505,12 @@
       <c r="Q147">
         <v>1</v>
       </c>
+      <c r="AG147" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>10</v>
       </c>
@@ -19975,8 +20562,12 @@
       <c r="Q148">
         <v>0</v>
       </c>
+      <c r="AG148" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>10</v>
       </c>
@@ -20028,8 +20619,12 @@
       <c r="Q149">
         <v>0</v>
       </c>
+      <c r="AG149" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>11</v>
       </c>
@@ -20081,8 +20676,12 @@
       <c r="Q150">
         <v>1</v>
       </c>
+      <c r="AG150" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>11</v>
       </c>
@@ -20134,8 +20733,12 @@
       <c r="Q151">
         <v>0</v>
       </c>
+      <c r="AG151" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>11</v>
       </c>
@@ -20187,8 +20790,12 @@
       <c r="Q152">
         <v>1</v>
       </c>
+      <c r="AG152" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>11</v>
       </c>
@@ -20240,8 +20847,12 @@
       <c r="Q153">
         <v>1</v>
       </c>
+      <c r="AG153" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>11</v>
       </c>
@@ -20293,8 +20904,12 @@
       <c r="Q154">
         <v>0</v>
       </c>
+      <c r="AG154" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>11</v>
       </c>
@@ -20346,8 +20961,12 @@
       <c r="Q155">
         <v>1</v>
       </c>
+      <c r="AG155" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>11</v>
       </c>
@@ -20399,8 +21018,12 @@
       <c r="Q156">
         <v>1</v>
       </c>
+      <c r="AG156" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>11</v>
       </c>
@@ -20452,8 +21075,12 @@
       <c r="Q157">
         <v>1</v>
       </c>
+      <c r="AG157" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>11</v>
       </c>
@@ -20505,8 +21132,12 @@
       <c r="Q158">
         <v>1</v>
       </c>
+      <c r="AG158" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>11</v>
       </c>
@@ -20558,8 +21189,12 @@
       <c r="Q159">
         <v>0</v>
       </c>
+      <c r="AG159" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>11</v>
       </c>
@@ -20611,8 +21246,12 @@
       <c r="Q160">
         <v>0</v>
       </c>
+      <c r="AG160" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>11</v>
       </c>
@@ -20664,8 +21303,12 @@
       <c r="Q161">
         <v>1</v>
       </c>
+      <c r="AG161" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>11</v>
       </c>
@@ -20717,8 +21360,12 @@
       <c r="Q162">
         <v>1</v>
       </c>
+      <c r="AG162" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="163" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>12</v>
       </c>
@@ -20770,8 +21417,12 @@
       <c r="Q163">
         <v>1</v>
       </c>
+      <c r="AG163" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>12</v>
       </c>
@@ -20823,8 +21474,12 @@
       <c r="Q164">
         <v>1</v>
       </c>
+      <c r="AG164" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>12</v>
       </c>
@@ -20876,8 +21531,12 @@
       <c r="Q165">
         <v>1</v>
       </c>
+      <c r="AG165" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>12</v>
       </c>
@@ -20929,8 +21588,12 @@
       <c r="Q166">
         <v>1</v>
       </c>
+      <c r="AG166" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>12</v>
       </c>
@@ -20982,8 +21645,12 @@
       <c r="Q167">
         <v>1</v>
       </c>
+      <c r="AG167" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>12</v>
       </c>
@@ -21035,8 +21702,12 @@
       <c r="Q168">
         <v>0</v>
       </c>
+      <c r="AG168" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>12</v>
       </c>
@@ -21088,8 +21759,12 @@
       <c r="Q169">
         <v>0</v>
       </c>
+      <c r="AG169" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>12</v>
       </c>
@@ -21141,8 +21816,12 @@
       <c r="Q170">
         <v>1</v>
       </c>
+      <c r="AG170" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>12</v>
       </c>
@@ -21194,8 +21873,12 @@
       <c r="Q171">
         <v>1</v>
       </c>
+      <c r="AG171" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>12</v>
       </c>
@@ -21247,8 +21930,12 @@
       <c r="Q172">
         <v>1</v>
       </c>
+      <c r="AG172" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>12</v>
       </c>
@@ -21300,8 +21987,12 @@
       <c r="Q173">
         <v>1</v>
       </c>
+      <c r="AG173" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>12</v>
       </c>
@@ -21353,8 +22044,12 @@
       <c r="Q174">
         <v>1</v>
       </c>
+      <c r="AG174" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>12</v>
       </c>
@@ -21406,8 +22101,12 @@
       <c r="Q175">
         <v>0</v>
       </c>
+      <c r="AG175" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>12</v>
       </c>
@@ -21459,8 +22158,12 @@
       <c r="Q176">
         <v>1</v>
       </c>
+      <c r="AG176" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>12</v>
       </c>
@@ -21512,8 +22215,12 @@
       <c r="Q177">
         <v>1</v>
       </c>
+      <c r="AG177" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="178" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>13</v>
       </c>
@@ -21565,8 +22272,12 @@
       <c r="Q178">
         <v>0</v>
       </c>
+      <c r="AG178" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>13</v>
       </c>
@@ -21618,8 +22329,12 @@
       <c r="Q179">
         <v>0</v>
       </c>
+      <c r="AG179" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>13</v>
       </c>
@@ -21671,8 +22386,12 @@
       <c r="Q180">
         <v>1</v>
       </c>
+      <c r="AG180" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>13</v>
       </c>
@@ -21724,8 +22443,12 @@
       <c r="Q181">
         <v>1</v>
       </c>
+      <c r="AG181" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>13</v>
       </c>
@@ -21777,8 +22500,12 @@
       <c r="Q182">
         <v>0</v>
       </c>
+      <c r="AG182" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>13</v>
       </c>
@@ -21830,8 +22557,12 @@
       <c r="Q183">
         <v>1</v>
       </c>
+      <c r="AG183" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>13</v>
       </c>
@@ -21883,8 +22614,12 @@
       <c r="Q184">
         <v>0</v>
       </c>
+      <c r="AG184" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>13</v>
       </c>
@@ -21936,8 +22671,12 @@
       <c r="Q185">
         <v>1</v>
       </c>
+      <c r="AG185" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="186" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>13</v>
       </c>
@@ -21989,8 +22728,12 @@
       <c r="Q186">
         <v>0</v>
       </c>
+      <c r="AG186" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>13</v>
       </c>
@@ -22042,8 +22785,12 @@
       <c r="Q187">
         <v>0</v>
       </c>
+      <c r="AG187" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>13</v>
       </c>
@@ -22095,8 +22842,12 @@
       <c r="Q188">
         <v>0</v>
       </c>
+      <c r="AG188" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>13</v>
       </c>
@@ -22148,8 +22899,12 @@
       <c r="Q189">
         <v>1</v>
       </c>
+      <c r="AG189" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>13</v>
       </c>
@@ -22201,8 +22956,12 @@
       <c r="Q190">
         <v>1</v>
       </c>
+      <c r="AG190" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>13</v>
       </c>
@@ -22254,8 +23013,12 @@
       <c r="Q191">
         <v>1</v>
       </c>
+      <c r="AG191" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>13</v>
       </c>
@@ -22307,8 +23070,12 @@
       <c r="Q192">
         <v>1</v>
       </c>
+      <c r="AG192" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>13</v>
       </c>
@@ -22360,8 +23127,12 @@
       <c r="Q193">
         <v>1</v>
       </c>
+      <c r="AG193" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>14</v>
       </c>
@@ -22413,8 +23184,12 @@
       <c r="Q194">
         <v>1</v>
       </c>
+      <c r="AG194" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>14</v>
       </c>
@@ -22466,8 +23241,12 @@
       <c r="Q195">
         <v>0</v>
       </c>
+      <c r="AG195" t="str">
+        <f t="shared" ref="AG195:AG257" si="31">IF(OR(OR(AND(I195&gt;0.5, M195=1, N195=1), AND(I195&lt;0.5, M195=0, N195=1), AND(I195&gt;0.5, M195=0, N195=0), AND(I195&lt;0.5, M195=1, N195=0)), OR(AND(J195&gt;0.5, M195=1, O195=1), AND(J195&lt;0.5, M195=0, O195=1), AND(J195&gt;0.5, M195=0, O195=0), AND(J195&lt;0.5, M195=1, O195=0)), OR(AND(K195&gt;0.5, M195=1, P195=1), AND(K195&lt;0.5, M195=0, P195=1), AND(K195&gt;0.5, M195=0, P195=0), AND(K195&lt;0.5, M195=1, P195=0)), OR(AND(L195&gt;0.5, M195=1, Q195=1), AND(L195&lt;0.5, M195=0, Q195=1), AND(L195&gt;0.5, M195=0, Q195=0), AND(L195&lt;0.5, M195=1, Q195=0))), "", "XXX")</f>
+        <v/>
+      </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>14</v>
       </c>
@@ -22519,8 +23298,12 @@
       <c r="Q196">
         <v>0</v>
       </c>
+      <c r="AG196" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>14</v>
       </c>
@@ -22572,8 +23355,12 @@
       <c r="Q197">
         <v>0</v>
       </c>
+      <c r="AG197" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>14</v>
       </c>
@@ -22625,8 +23412,12 @@
       <c r="Q198">
         <v>1</v>
       </c>
+      <c r="AG198" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>14</v>
       </c>
@@ -22678,8 +23469,12 @@
       <c r="Q199">
         <v>0</v>
       </c>
+      <c r="AG199" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>14</v>
       </c>
@@ -22731,8 +23526,12 @@
       <c r="Q200">
         <v>1</v>
       </c>
+      <c r="AG200" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>14</v>
       </c>
@@ -22784,8 +23583,12 @@
       <c r="Q201">
         <v>0</v>
       </c>
+      <c r="AG201" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>14</v>
       </c>
@@ -22837,8 +23640,12 @@
       <c r="Q202">
         <v>1</v>
       </c>
+      <c r="AG202" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="203" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>14</v>
       </c>
@@ -22890,8 +23697,12 @@
       <c r="Q203">
         <v>0</v>
       </c>
+      <c r="AG203" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>14</v>
       </c>
@@ -22943,8 +23754,12 @@
       <c r="Q204">
         <v>1</v>
       </c>
+      <c r="AG204" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>14</v>
       </c>
@@ -22996,8 +23811,12 @@
       <c r="Q205">
         <v>0</v>
       </c>
+      <c r="AG205" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>14</v>
       </c>
@@ -23049,8 +23868,12 @@
       <c r="Q206">
         <v>1</v>
       </c>
+      <c r="AG206" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>14</v>
       </c>
@@ -23102,8 +23925,12 @@
       <c r="Q207">
         <v>1</v>
       </c>
+      <c r="AG207" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>14</v>
       </c>
@@ -23155,8 +23982,12 @@
       <c r="Q208">
         <v>0</v>
       </c>
+      <c r="AG208" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>14</v>
       </c>
@@ -23208,8 +24039,12 @@
       <c r="Q209">
         <v>1</v>
       </c>
+      <c r="AG209" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>15</v>
       </c>
@@ -23261,8 +24096,12 @@
       <c r="Q210">
         <v>0</v>
       </c>
+      <c r="AG210" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>15</v>
       </c>
@@ -23314,8 +24153,12 @@
       <c r="Q211">
         <v>0</v>
       </c>
+      <c r="AG211" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="212" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>15</v>
       </c>
@@ -23367,8 +24210,12 @@
       <c r="Q212">
         <v>1</v>
       </c>
+      <c r="AG212" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>15</v>
       </c>
@@ -23420,8 +24267,12 @@
       <c r="Q213">
         <v>1</v>
       </c>
+      <c r="AG213" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>15</v>
       </c>
@@ -23473,8 +24324,12 @@
       <c r="Q214">
         <v>1</v>
       </c>
+      <c r="AG214" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>15</v>
       </c>
@@ -23526,8 +24381,12 @@
       <c r="Q215">
         <v>1</v>
       </c>
+      <c r="AG215" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>15</v>
       </c>
@@ -23579,8 +24438,12 @@
       <c r="Q216">
         <v>1</v>
       </c>
+      <c r="AG216" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>15</v>
       </c>
@@ -23632,8 +24495,12 @@
       <c r="Q217">
         <v>1</v>
       </c>
+      <c r="AG217" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>15</v>
       </c>
@@ -23685,8 +24552,12 @@
       <c r="Q218">
         <v>1</v>
       </c>
+      <c r="AG218" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>15</v>
       </c>
@@ -23738,8 +24609,12 @@
       <c r="Q219">
         <v>0</v>
       </c>
+      <c r="AG219" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>15</v>
       </c>
@@ -23791,8 +24666,12 @@
       <c r="Q220">
         <v>1</v>
       </c>
+      <c r="AG220" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="221" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>15</v>
       </c>
@@ -23844,8 +24723,12 @@
       <c r="Q221">
         <v>0</v>
       </c>
+      <c r="AG221" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>15</v>
       </c>
@@ -23897,8 +24780,12 @@
       <c r="Q222">
         <v>0</v>
       </c>
+      <c r="AG222" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>15</v>
       </c>
@@ -23950,8 +24837,12 @@
       <c r="Q223">
         <v>1</v>
       </c>
+      <c r="AG223" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>15</v>
       </c>
@@ -24003,8 +24894,12 @@
       <c r="Q224">
         <v>0</v>
       </c>
+      <c r="AG224" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>15</v>
       </c>
@@ -24056,8 +24951,12 @@
       <c r="Q225">
         <v>1</v>
       </c>
+      <c r="AG225" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>16</v>
       </c>
@@ -24109,8 +25008,12 @@
       <c r="Q226">
         <v>1</v>
       </c>
+      <c r="AG226" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>16</v>
       </c>
@@ -24162,8 +25065,12 @@
       <c r="Q227">
         <v>0</v>
       </c>
+      <c r="AG227" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>16</v>
       </c>
@@ -24215,8 +25122,12 @@
       <c r="Q228">
         <v>0</v>
       </c>
+      <c r="AG228" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>16</v>
       </c>
@@ -24268,8 +25179,12 @@
       <c r="Q229">
         <v>1</v>
       </c>
+      <c r="AG229" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="230" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>16</v>
       </c>
@@ -24321,8 +25236,12 @@
       <c r="Q230">
         <v>1</v>
       </c>
+      <c r="AG230" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>16</v>
       </c>
@@ -24374,8 +25293,12 @@
       <c r="Q231">
         <v>1</v>
       </c>
+      <c r="AG231" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>16</v>
       </c>
@@ -24427,8 +25350,12 @@
       <c r="Q232">
         <v>1</v>
       </c>
+      <c r="AG232" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>16</v>
       </c>
@@ -24480,8 +25407,12 @@
       <c r="Q233">
         <v>0</v>
       </c>
+      <c r="AG233" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>16</v>
       </c>
@@ -24533,8 +25464,12 @@
       <c r="Q234">
         <v>1</v>
       </c>
+      <c r="AG234" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>16</v>
       </c>
@@ -24586,8 +25521,12 @@
       <c r="Q235">
         <v>1</v>
       </c>
+      <c r="AG235" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>16</v>
       </c>
@@ -24639,8 +25578,12 @@
       <c r="Q236">
         <v>1</v>
       </c>
+      <c r="AG236" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>16</v>
       </c>
@@ -24692,8 +25635,12 @@
       <c r="Q237">
         <v>1</v>
       </c>
+      <c r="AG237" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="238" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>16</v>
       </c>
@@ -24745,8 +25692,12 @@
       <c r="Q238">
         <v>1</v>
       </c>
+      <c r="AG238" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>16</v>
       </c>
@@ -24798,8 +25749,12 @@
       <c r="Q239">
         <v>1</v>
       </c>
+      <c r="AG239" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>16</v>
       </c>
@@ -24851,8 +25806,12 @@
       <c r="Q240">
         <v>0</v>
       </c>
+      <c r="AG240" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="241" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>16</v>
       </c>
@@ -24904,8 +25863,12 @@
       <c r="Q241">
         <v>0</v>
       </c>
+      <c r="AG241" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="242" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>17</v>
       </c>
@@ -24957,8 +25920,12 @@
       <c r="Q242">
         <v>1</v>
       </c>
+      <c r="AG242" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="243" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>17</v>
       </c>
@@ -25010,8 +25977,12 @@
       <c r="Q243">
         <v>1</v>
       </c>
+      <c r="AG243" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="244" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>17</v>
       </c>
@@ -25063,8 +26034,12 @@
       <c r="Q244">
         <v>0</v>
       </c>
+      <c r="AG244" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="245" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>17</v>
       </c>
@@ -25116,8 +26091,12 @@
       <c r="Q245">
         <v>1</v>
       </c>
+      <c r="AG245" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="246" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>17</v>
       </c>
@@ -25169,8 +26148,12 @@
       <c r="Q246">
         <v>1</v>
       </c>
+      <c r="AG246" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="247" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>17</v>
       </c>
@@ -25222,8 +26205,12 @@
       <c r="Q247">
         <v>0</v>
       </c>
+      <c r="AG247" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="248" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>17</v>
       </c>
@@ -25275,8 +26262,12 @@
       <c r="Q248">
         <v>1</v>
       </c>
+      <c r="AG248" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="249" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>17</v>
       </c>
@@ -25328,8 +26319,12 @@
       <c r="Q249">
         <v>0</v>
       </c>
+      <c r="AG249" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="250" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>17</v>
       </c>
@@ -25381,8 +26376,12 @@
       <c r="Q250">
         <v>0</v>
       </c>
+      <c r="AG250" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="251" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>17</v>
       </c>
@@ -25434,8 +26433,12 @@
       <c r="Q251">
         <v>1</v>
       </c>
+      <c r="AG251" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="252" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>17</v>
       </c>
@@ -25487,8 +26490,12 @@
       <c r="Q252">
         <v>1</v>
       </c>
+      <c r="AG252" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="253" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>17</v>
       </c>
@@ -25540,8 +26547,12 @@
       <c r="Q253">
         <v>1</v>
       </c>
+      <c r="AG253" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="254" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>17</v>
       </c>
@@ -25593,8 +26604,12 @@
       <c r="Q254">
         <v>1</v>
       </c>
+      <c r="AG254" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="255" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>17</v>
       </c>
@@ -25646,8 +26661,12 @@
       <c r="Q255">
         <v>1</v>
       </c>
+      <c r="AG255" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="256" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>17</v>
       </c>
@@ -25699,8 +26718,12 @@
       <c r="Q256">
         <v>1</v>
       </c>
+      <c r="AG256" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="257" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>17</v>
       </c>
@@ -25752,8 +26775,12 @@
       <c r="Q257">
         <v>1</v>
       </c>
+      <c r="AG257" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
     </row>
-    <row r="258" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="N258" s="2">
         <f>SUM(N2:N257)</f>
         <v>151</v>
@@ -25764,14 +26791,14 @@
       </c>
       <c r="P258" s="2">
         <f>SUM(P2:P257)</f>
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="Q258" s="2">
         <f>SUM(Q2:Q257)</f>
         <v>165</v>
       </c>
     </row>
-    <row r="259" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="259" spans="1:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding and editing charts
</commit_message>
<xml_diff>
--- a/AMOS 2018 SEASON OUTPUT DRAFT 20180103.xlsx
+++ b/AMOS 2018 SEASON OUTPUT DRAFT 20180103.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\Documents\SportsAnalytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4981D850-0860-40FD-919D-F366DE8D05F4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5702BA1E-AFF1-4CEA-BB4E-0D6F2ABA2063}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMOS 2018 SEASON OUTPUT DRAFT 2" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="153">
   <si>
     <t>WEEK</t>
   </si>
@@ -486,6 +486,9 @@
   <si>
     <t>Ranges</t>
   </si>
+  <si>
+    <t>AVERAGE_WEEKLY</t>
+  </si>
 </sst>
 </file>
 
@@ -808,7 +811,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -952,17 +955,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1008,7 +1000,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="17"/>
@@ -1031,9 +1023,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1083,6 +1074,15 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF8F45C7"/>
+      <color rgb="FFFF5050"/>
+      <color rgb="FFA86ED4"/>
+      <color rgb="FFED7D31"/>
+      <color rgb="FFFF6600"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2435,6 +2435,8 @@
         <c:axId val="536352632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.85000000000000009"/>
+          <c:min val="0.4"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -6463,6 +6465,767 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'AMOS 2018 SEASON OUTPUT DRAFT 2'!$AB$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AVERAGE_WEEKLY</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="bg2">
+                <a:lumMod val="25000"/>
+                <a:alpha val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>'AMOS 2018 SEASON OUTPUT DRAFT 2'!$AB$2:$AB$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>9.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7.75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-2ED7-42F9-8F13-F7E7E9ACEE24}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="485201544"/>
+        <c:axId val="485202200"/>
+      </c:areaChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'AMOS 2018 SEASON OUTPUT DRAFT 2'!$S$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AMOS_WEEKLY_SUM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'AMOS 2018 SEASON OUTPUT DRAFT 2'!$S$2:$S$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2ED7-42F9-8F13-F7E7E9ACEE24}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'AMOS 2018 SEASON OUTPUT DRAFT 2'!$T$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ELO_WEEKLY_SUM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="ED7D31">
+                  <a:alpha val="83137"/>
+                </a:srgbClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF6600"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'AMOS 2018 SEASON OUTPUT DRAFT 2'!$T$2:$T$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2ED7-42F9-8F13-F7E7E9ACEE24}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'AMOS 2018 SEASON OUTPUT DRAFT 2'!$U$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BING_WEEKLY-SUM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'AMOS 2018 SEASON OUTPUT DRAFT 2'!$U$2:$U$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-2ED7-42F9-8F13-F7E7E9ACEE24}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'AMOS 2018 SEASON OUTPUT DRAFT 2'!$V$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FPI_WEEKLY_SUM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="A86ED4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="8F45C7"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'AMOS 2018 SEASON OUTPUT DRAFT 2'!$V$2:$V$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-2ED7-42F9-8F13-F7E7E9ACEE24}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="485201544"/>
+        <c:axId val="485202200"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="485201544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="485202200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="485202200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="485201544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -6704,6 +7467,46 @@
 </file>
 
 <file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -10290,6 +11093,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -10446,16 +11752,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>97</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>448235</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>22410</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>457759</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>31935</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10484,16 +11790,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>118223</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>24653</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
-      <xdr:row>95</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>108697</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>24653</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10553,6 +11859,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>582706</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41EADC60-C111-415B-A677-482C69E801A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10860,8 +12204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z38" sqref="Z38"/>
+    <sheetView topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10975,6 +12319,9 @@
       <c r="AA1" t="s">
         <v>127</v>
       </c>
+      <c r="AB1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -11067,6 +12414,10 @@
         <f>SUM(V2/W2)</f>
         <v>0.5</v>
       </c>
+      <c r="AB2">
+        <f>AVERAGE(S2:V2)</f>
+        <v>9.25</v>
+      </c>
       <c r="AG2" t="str">
         <f>IF(OR(OR(AND(I2&gt;0.5, M2=1, N2=1), AND(I2&lt;0.5, M2=0, N2=1), AND(I2&gt;0.5, M2=0, N2=0), AND(I2&lt;0.5, M2=1, N2=0)), OR(AND(J2&gt;0.5, M2=1, O2=1), AND(J2&lt;0.5, M2=0, O2=1), AND(J2&gt;0.5, M2=0, O2=0), AND(J2&lt;0.5, M2=1, O2=0)), OR(AND(K2&gt;0.5, M2=1, P2=1), AND(K2&lt;0.5, M2=0, P2=1), AND(K2&gt;0.5, M2=0, P2=0), AND(K2&lt;0.5, M2=1, P2=0)), OR(AND(L2&gt;0.5, M2=1, Q2=1), AND(L2&lt;0.5, M2=0, Q2=1), AND(L2&gt;0.5, M2=0, Q2=0), AND(L2&lt;0.5, M2=1, Q2=0))), "", "XXX")</f>
         <v/>
@@ -11163,8 +12514,12 @@
         <f t="shared" ref="AA3:AA18" si="5">SUM(V3/W3)</f>
         <v>0.625</v>
       </c>
+      <c r="AB3">
+        <f t="shared" ref="AB3:AB18" si="6">AVERAGE(S3:V3)</f>
+        <v>9</v>
+      </c>
       <c r="AG3" t="str">
-        <f t="shared" ref="AG3:AG66" si="6">IF(OR(OR(AND(I3&gt;0.5, M3=1, N3=1), AND(I3&lt;0.5, M3=0, N3=1), AND(I3&gt;0.5, M3=0, N3=0), AND(I3&lt;0.5, M3=1, N3=0)), OR(AND(J3&gt;0.5, M3=1, O3=1), AND(J3&lt;0.5, M3=0, O3=1), AND(J3&gt;0.5, M3=0, O3=0), AND(J3&lt;0.5, M3=1, O3=0)), OR(AND(K3&gt;0.5, M3=1, P3=1), AND(K3&lt;0.5, M3=0, P3=1), AND(K3&gt;0.5, M3=0, P3=0), AND(K3&lt;0.5, M3=1, P3=0)), OR(AND(L3&gt;0.5, M3=1, Q3=1), AND(L3&lt;0.5, M3=0, Q3=1), AND(L3&gt;0.5, M3=0, Q3=0), AND(L3&lt;0.5, M3=1, Q3=0))), "", "XXX")</f>
+        <f t="shared" ref="AG3:AG66" si="7">IF(OR(OR(AND(I3&gt;0.5, M3=1, N3=1), AND(I3&lt;0.5, M3=0, N3=1), AND(I3&gt;0.5, M3=0, N3=0), AND(I3&lt;0.5, M3=1, N3=0)), OR(AND(J3&gt;0.5, M3=1, O3=1), AND(J3&lt;0.5, M3=0, O3=1), AND(J3&gt;0.5, M3=0, O3=0), AND(J3&lt;0.5, M3=1, O3=0)), OR(AND(K3&gt;0.5, M3=1, P3=1), AND(K3&lt;0.5, M3=0, P3=1), AND(K3&gt;0.5, M3=0, P3=0), AND(K3&lt;0.5, M3=1, P3=0)), OR(AND(L3&gt;0.5, M3=1, Q3=1), AND(L3&lt;0.5, M3=0, Q3=1), AND(L3&gt;0.5, M3=0, Q3=0), AND(L3&lt;0.5, M3=1, Q3=0))), "", "XXX")</f>
         <v/>
       </c>
     </row>
@@ -11228,15 +12583,15 @@
         <v>10</v>
       </c>
       <c r="T4">
-        <f t="shared" ref="T4:V4" si="7">SUM(O34:O49)</f>
+        <f t="shared" ref="T4:V4" si="8">SUM(O34:O49)</f>
         <v>8</v>
       </c>
       <c r="U4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="V4">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="W4">
@@ -11259,8 +12614,12 @@
         <f t="shared" si="5"/>
         <v>0.6875</v>
       </c>
+      <c r="AB4">
+        <f t="shared" si="6"/>
+        <v>9.75</v>
+      </c>
       <c r="AG4" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>XXX</v>
       </c>
     </row>
@@ -11324,15 +12683,15 @@
         <v>8</v>
       </c>
       <c r="T5">
-        <f t="shared" ref="T5:V5" si="8">SUM(O50:O64)</f>
+        <f t="shared" ref="T5:V5" si="9">SUM(O50:O64)</f>
         <v>11</v>
       </c>
       <c r="U5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="V5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="W5">
@@ -11355,8 +12714,12 @@
         <f t="shared" si="5"/>
         <v>0.73333333333333328</v>
       </c>
+      <c r="AB5">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
       <c r="AG5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -11420,15 +12783,15 @@
         <v>7</v>
       </c>
       <c r="T6">
-        <f t="shared" ref="T6:V6" si="9">SUM(O65:O79)</f>
+        <f t="shared" ref="T6:V6" si="10">SUM(O65:O79)</f>
         <v>10</v>
       </c>
       <c r="U6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="V6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
       <c r="W6">
@@ -11451,8 +12814,12 @@
         <f t="shared" si="5"/>
         <v>0.66666666666666663</v>
       </c>
+      <c r="AB6">
+        <f t="shared" si="6"/>
+        <v>9.25</v>
+      </c>
       <c r="AG6" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -11516,15 +12883,15 @@
         <v>11</v>
       </c>
       <c r="T7">
-        <f t="shared" ref="T7:V7" si="10">SUM(O80:O94)</f>
+        <f t="shared" ref="T7:V7" si="11">SUM(O80:O94)</f>
         <v>11</v>
       </c>
       <c r="U7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="V7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
       <c r="W7">
@@ -11547,8 +12914,12 @@
         <f t="shared" si="5"/>
         <v>0.73333333333333328</v>
       </c>
+      <c r="AB7">
+        <f t="shared" si="6"/>
+        <v>11</v>
+      </c>
       <c r="AG7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -11612,15 +12983,15 @@
         <v>8</v>
       </c>
       <c r="T8">
-        <f t="shared" ref="T8:V8" si="11">SUM(O95:O108)</f>
+        <f t="shared" ref="T8:V8" si="12">SUM(O95:O108)</f>
         <v>8</v>
       </c>
       <c r="U8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11</v>
       </c>
       <c r="V8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="W8">
@@ -11643,8 +13014,12 @@
         <f t="shared" si="5"/>
         <v>0.5714285714285714</v>
       </c>
+      <c r="AB8">
+        <f t="shared" si="6"/>
+        <v>8.75</v>
+      </c>
       <c r="AG8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -11708,15 +13083,15 @@
         <v>8</v>
       </c>
       <c r="T9">
-        <f t="shared" ref="T9:V9" si="12">SUM(O109:O122)</f>
+        <f t="shared" ref="T9:V9" si="13">SUM(O109:O122)</f>
         <v>11</v>
       </c>
       <c r="U9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>11</v>
       </c>
       <c r="V9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>9</v>
       </c>
       <c r="W9">
@@ -11739,8 +13114,12 @@
         <f t="shared" si="5"/>
         <v>0.6428571428571429</v>
       </c>
+      <c r="AB9">
+        <f t="shared" si="6"/>
+        <v>9.75</v>
+      </c>
       <c r="AG9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -11804,15 +13183,15 @@
         <v>6</v>
       </c>
       <c r="T10">
-        <f t="shared" ref="T10:V10" si="13">SUM(O123:O135)</f>
+        <f t="shared" ref="T10:V10" si="14">SUM(O123:O135)</f>
         <v>8</v>
       </c>
       <c r="U10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="V10">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="W10">
@@ -11835,8 +13214,12 @@
         <f t="shared" si="5"/>
         <v>0.61538461538461542</v>
       </c>
+      <c r="AB10">
+        <f t="shared" si="6"/>
+        <v>7.5</v>
+      </c>
       <c r="AG10" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -11900,15 +13283,15 @@
         <v>10</v>
       </c>
       <c r="T11">
-        <f t="shared" ref="T11:V11" si="14">SUM(O136:O149)</f>
+        <f t="shared" ref="T11:V11" si="15">SUM(O136:O149)</f>
         <v>8</v>
       </c>
       <c r="U11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="V11">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>8</v>
       </c>
       <c r="W11">
@@ -11931,8 +13314,12 @@
         <f t="shared" si="5"/>
         <v>0.5714285714285714</v>
       </c>
+      <c r="AB11">
+        <f t="shared" si="6"/>
+        <v>8.5</v>
+      </c>
       <c r="AG11" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -11996,15 +13383,15 @@
         <v>6</v>
       </c>
       <c r="T12">
-        <f t="shared" ref="T12:V12" si="15">SUM(O150:O162)</f>
+        <f t="shared" ref="T12:V12" si="16">SUM(O150:O162)</f>
         <v>7</v>
       </c>
       <c r="U12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>8</v>
       </c>
       <c r="V12">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9</v>
       </c>
       <c r="W12">
@@ -12027,8 +13414,12 @@
         <f t="shared" si="5"/>
         <v>0.69230769230769229</v>
       </c>
+      <c r="AB12">
+        <f t="shared" si="6"/>
+        <v>7.5</v>
+      </c>
       <c r="AG12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -12092,15 +13483,15 @@
         <v>12</v>
       </c>
       <c r="T13">
-        <f t="shared" ref="T13:V13" si="16">SUM(O163:O177)</f>
+        <f t="shared" ref="T13:V13" si="17">SUM(O163:O177)</f>
         <v>12</v>
       </c>
       <c r="U13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>11</v>
       </c>
       <c r="V13">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>12</v>
       </c>
       <c r="W13">
@@ -12123,8 +13514,12 @@
         <f t="shared" si="5"/>
         <v>0.8</v>
       </c>
+      <c r="AB13">
+        <f t="shared" si="6"/>
+        <v>11.75</v>
+      </c>
       <c r="AG13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -12188,15 +13583,15 @@
         <v>10</v>
       </c>
       <c r="T14">
-        <f t="shared" ref="T14:V14" si="17">SUM(O178:O193)</f>
+        <f t="shared" ref="T14:V14" si="18">SUM(O178:O193)</f>
         <v>8</v>
       </c>
       <c r="U14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
       <c r="V14">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="W14">
@@ -12219,8 +13614,12 @@
         <f t="shared" si="5"/>
         <v>0.5625</v>
       </c>
+      <c r="AB14">
+        <f t="shared" si="6"/>
+        <v>9.25</v>
+      </c>
       <c r="AG14" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -12284,15 +13683,15 @@
         <v>7</v>
       </c>
       <c r="T15">
-        <f t="shared" ref="T15:V15" si="18">SUM(O194:O209)</f>
+        <f t="shared" ref="T15:V15" si="19">SUM(O194:O209)</f>
         <v>7</v>
       </c>
       <c r="U15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9</v>
       </c>
       <c r="V15">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>8</v>
       </c>
       <c r="W15">
@@ -12315,8 +13714,12 @@
         <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
+      <c r="AB15">
+        <f t="shared" si="6"/>
+        <v>7.75</v>
+      </c>
       <c r="AG15" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -12380,15 +13783,15 @@
         <v>7</v>
       </c>
       <c r="T16">
-        <f t="shared" ref="T16:V16" si="19">SUM(O210:O225)</f>
+        <f t="shared" ref="T16:V16" si="20">SUM(O210:O225)</f>
         <v>9</v>
       </c>
       <c r="U16">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9</v>
       </c>
       <c r="V16">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>10</v>
       </c>
       <c r="W16">
@@ -12411,8 +13814,12 @@
         <f t="shared" si="5"/>
         <v>0.625</v>
       </c>
+      <c r="AB16">
+        <f t="shared" si="6"/>
+        <v>8.75</v>
+      </c>
       <c r="AG16" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -12476,15 +13883,15 @@
         <v>11</v>
       </c>
       <c r="T17">
-        <f t="shared" ref="T17:V17" si="20">SUM(O226:O241)</f>
+        <f t="shared" ref="T17:V17" si="21">SUM(O226:O241)</f>
         <v>11</v>
       </c>
       <c r="U17">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>9</v>
       </c>
       <c r="V17">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>11</v>
       </c>
       <c r="W17">
@@ -12507,8 +13914,12 @@
         <f t="shared" si="5"/>
         <v>0.6875</v>
       </c>
+      <c r="AB17">
+        <f t="shared" si="6"/>
+        <v>10.5</v>
+      </c>
       <c r="AG17" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -12572,15 +13983,15 @@
         <v>12</v>
       </c>
       <c r="T18">
-        <f t="shared" ref="T18:V18" si="21">SUM(O242:O257)</f>
+        <f t="shared" ref="T18:V18" si="22">SUM(O242:O257)</f>
         <v>12</v>
       </c>
       <c r="U18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>11</v>
       </c>
       <c r="V18">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>12</v>
       </c>
       <c r="W18">
@@ -12603,8 +14014,12 @@
         <f t="shared" si="5"/>
         <v>0.75</v>
       </c>
+      <c r="AB18">
+        <f t="shared" si="6"/>
+        <v>11.75</v>
+      </c>
       <c r="AG18" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -12668,15 +14083,15 @@
         <v>8.882352941176471</v>
       </c>
       <c r="T19" s="2">
-        <f t="shared" ref="T19:V19" si="22">AVERAGE(T2:T18)</f>
+        <f t="shared" ref="T19:V19" si="23">AVERAGE(T2:T18)</f>
         <v>9.3529411764705888</v>
       </c>
       <c r="U19" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>9.7058823529411757</v>
       </c>
       <c r="V19" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>9.7058823529411757</v>
       </c>
       <c r="X19" s="5">
@@ -12684,19 +14099,19 @@
         <v>0.58829724197371247</v>
       </c>
       <c r="Y19" s="5">
-        <f t="shared" ref="Y19:AA19" si="23">AVERAGE(Y2:Y18)</f>
+        <f t="shared" ref="Y19:AA19" si="24">AVERAGE(Y2:Y18)</f>
         <v>0.62225005386770083</v>
       </c>
       <c r="Z19" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.64624272786037484</v>
       </c>
       <c r="AA19" s="5">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0.64495528980823102</v>
       </c>
       <c r="AG19" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -12757,19 +14172,19 @@
         <v>151</v>
       </c>
       <c r="T20">
-        <f t="shared" ref="T20:V20" si="24">SUM(T2:T18)</f>
+        <f t="shared" ref="T20:V20" si="25">SUM(T2:T18)</f>
         <v>159</v>
       </c>
       <c r="U20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>165</v>
       </c>
       <c r="V20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>165</v>
       </c>
       <c r="AG20" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -12826,7 +14241,7 @@
         <v>0</v>
       </c>
       <c r="AG21" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -12883,7 +14298,7 @@
         <v>1</v>
       </c>
       <c r="AG22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -12940,7 +14355,7 @@
         <v>0</v>
       </c>
       <c r="AG23" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -12999,7 +14414,7 @@
       <c r="R24" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="S24" s="12" t="s">
+      <c r="S24" s="7" t="s">
         <v>137</v>
       </c>
       <c r="T24" s="7" t="s">
@@ -13036,7 +14451,7 @@
         <v>148</v>
       </c>
       <c r="AG24" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -13092,7 +14507,7 @@
       <c r="Q25">
         <v>0</v>
       </c>
-      <c r="R25" s="14" t="s">
+      <c r="R25" s="13" t="s">
         <v>130</v>
       </c>
       <c r="S25">
@@ -13116,7 +14531,7 @@
         <v>2</v>
       </c>
       <c r="X25">
-        <f t="shared" ref="X25:X32" si="25">SUM(V25/W25)</f>
+        <f t="shared" ref="X25:X32" si="26">SUM(V25/W25)</f>
         <v>1</v>
       </c>
       <c r="Y25">
@@ -13127,7 +14542,7 @@
         <f>COUNTIFS(K2:K257,"&gt;=0.0",K2:K257,"&lt;0.2")</f>
         <v>0</v>
       </c>
-      <c r="AA25" s="13" t="s">
+      <c r="AA25" s="12" t="s">
         <v>149</v>
       </c>
       <c r="AB25">
@@ -13139,11 +14554,11 @@
         <v>3</v>
       </c>
       <c r="AD25">
-        <f t="shared" ref="AD25:AD32" si="26">SUM(AB25/AC25)</f>
+        <f t="shared" ref="AD25:AD32" si="27">SUM(AB25/AC25)</f>
         <v>1</v>
       </c>
       <c r="AG25" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -13199,7 +14614,7 @@
       <c r="Q26">
         <v>1</v>
       </c>
-      <c r="R26" s="14" t="s">
+      <c r="R26" s="13" t="s">
         <v>129</v>
       </c>
       <c r="S26">
@@ -13223,7 +14638,7 @@
         <v>13</v>
       </c>
       <c r="X26">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.53846153846153844</v>
       </c>
       <c r="Y26">
@@ -13235,7 +14650,7 @@
         <v>21</v>
       </c>
       <c r="AA26">
-        <f t="shared" ref="AA26:AA32" si="27">SUM(Y26/Z26)</f>
+        <f t="shared" ref="AA26:AA32" si="28">SUM(Y26/Z26)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="AB26">
@@ -13247,11 +14662,11 @@
         <v>12</v>
       </c>
       <c r="AD26">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.75</v>
       </c>
       <c r="AG26" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -13307,7 +14722,7 @@
       <c r="Q27">
         <v>0</v>
       </c>
-      <c r="R27" s="14" t="s">
+      <c r="R27" s="13" t="s">
         <v>131</v>
       </c>
       <c r="S27">
@@ -13319,7 +14734,7 @@
         <v>47</v>
       </c>
       <c r="U27">
-        <f t="shared" ref="U27:U32" si="28">SUM(S27/T27)</f>
+        <f t="shared" ref="U27:U32" si="29">SUM(S27/T27)</f>
         <v>0.55319148936170215</v>
       </c>
       <c r="V27">
@@ -13331,7 +14746,7 @@
         <v>27</v>
       </c>
       <c r="X27">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.59259259259259256</v>
       </c>
       <c r="Y27">
@@ -13343,7 +14758,7 @@
         <v>22</v>
       </c>
       <c r="AA27">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.59090909090909094</v>
       </c>
       <c r="AB27">
@@ -13355,11 +14770,11 @@
         <v>23</v>
       </c>
       <c r="AD27">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.52173913043478259</v>
       </c>
       <c r="AG27" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -13415,7 +14830,7 @@
       <c r="Q28">
         <v>1</v>
       </c>
-      <c r="R28" s="14" t="s">
+      <c r="R28" s="13" t="s">
         <v>132</v>
       </c>
       <c r="S28">
@@ -13427,7 +14842,7 @@
         <v>41</v>
       </c>
       <c r="U28">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.41463414634146339</v>
       </c>
       <c r="V28">
@@ -13439,7 +14854,7 @@
         <v>28</v>
       </c>
       <c r="X28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.42857142857142855</v>
       </c>
       <c r="Y28">
@@ -13451,7 +14866,7 @@
         <v>33</v>
       </c>
       <c r="AA28">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.48484848484848486</v>
       </c>
       <c r="AB28">
@@ -13463,11 +14878,11 @@
         <v>35</v>
       </c>
       <c r="AD28">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.51428571428571423</v>
       </c>
       <c r="AG28" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -13523,7 +14938,7 @@
       <c r="Q29">
         <v>1</v>
       </c>
-      <c r="R29" s="14" t="s">
+      <c r="R29" s="13" t="s">
         <v>133</v>
       </c>
       <c r="S29">
@@ -13535,7 +14950,7 @@
         <v>25</v>
       </c>
       <c r="U29">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="V29">
@@ -13547,7 +14962,7 @@
         <v>50</v>
       </c>
       <c r="X29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.56000000000000005</v>
       </c>
       <c r="Y29">
@@ -13559,7 +14974,7 @@
         <v>43</v>
       </c>
       <c r="AA29">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.48837209302325579</v>
       </c>
       <c r="AB29">
@@ -13571,11 +14986,11 @@
         <v>50</v>
       </c>
       <c r="AD29">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.46</v>
       </c>
       <c r="AG29" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -13631,7 +15046,7 @@
       <c r="Q30">
         <v>1</v>
       </c>
-      <c r="R30" s="8" t="s">
+      <c r="R30" s="13" t="s">
         <v>134</v>
       </c>
       <c r="S30">
@@ -13643,7 +15058,7 @@
         <v>44</v>
       </c>
       <c r="U30">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.63636363636363635</v>
       </c>
       <c r="V30">
@@ -13655,7 +15070,7 @@
         <v>70</v>
       </c>
       <c r="X30">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.6</v>
       </c>
       <c r="Y30">
@@ -13667,7 +15082,7 @@
         <v>85</v>
       </c>
       <c r="AA30">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.69411764705882351</v>
       </c>
       <c r="AB30">
@@ -13679,11 +15094,11 @@
         <v>53</v>
       </c>
       <c r="AD30">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.67924528301886788</v>
       </c>
       <c r="AG30" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -13739,7 +15154,7 @@
       <c r="Q31">
         <v>1</v>
       </c>
-      <c r="R31" s="14" t="s">
+      <c r="R31" s="13" t="s">
         <v>135</v>
       </c>
       <c r="S31">
@@ -13751,7 +15166,7 @@
         <v>47</v>
       </c>
       <c r="U31">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.78723404255319152</v>
       </c>
       <c r="V31">
@@ -13763,7 +15178,7 @@
         <v>41</v>
       </c>
       <c r="X31">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.70731707317073167</v>
       </c>
       <c r="Y31">
@@ -13775,7 +15190,7 @@
         <v>48</v>
       </c>
       <c r="AA31">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0.79166666666666663</v>
       </c>
       <c r="AB31">
@@ -13787,11 +15202,11 @@
         <v>53</v>
       </c>
       <c r="AD31">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.79245283018867929</v>
       </c>
       <c r="AG31" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -13847,7 +15262,7 @@
       <c r="Q32">
         <v>1</v>
       </c>
-      <c r="R32" s="14" t="s">
+      <c r="R32" s="13" t="s">
         <v>136</v>
       </c>
       <c r="S32">
@@ -13859,7 +15274,7 @@
         <v>36</v>
       </c>
       <c r="U32">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0.61111111111111116</v>
       </c>
       <c r="V32">
@@ -13871,7 +15286,7 @@
         <v>25</v>
       </c>
       <c r="X32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0.92</v>
       </c>
       <c r="Y32">
@@ -13883,7 +15298,7 @@
         <v>4</v>
       </c>
       <c r="AA32">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
       <c r="AB32">
@@ -13895,11 +15310,11 @@
         <v>27</v>
       </c>
       <c r="AD32">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0.81481481481481477</v>
       </c>
       <c r="AG32" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14007,7 +15422,7 @@
         <v>0.69156722159285733</v>
       </c>
       <c r="AG33" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14065,7 +15480,7 @@
       </c>
       <c r="R34" s="9"/>
       <c r="AG34" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14122,7 +15537,7 @@
         <v>0</v>
       </c>
       <c r="AG35" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14179,7 +15594,7 @@
         <v>1</v>
       </c>
       <c r="AG36" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14236,7 +15651,7 @@
         <v>1</v>
       </c>
       <c r="AG37" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14293,7 +15708,7 @@
         <v>0</v>
       </c>
       <c r="AG38" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14350,7 +15765,7 @@
         <v>0</v>
       </c>
       <c r="AG39" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14407,7 +15822,7 @@
         <v>1</v>
       </c>
       <c r="AG40" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14464,7 +15879,7 @@
         <v>1</v>
       </c>
       <c r="AG41" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14521,7 +15936,7 @@
         <v>0</v>
       </c>
       <c r="AG42" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14578,7 +15993,7 @@
         <v>1</v>
       </c>
       <c r="AG43" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14635,7 +16050,7 @@
         <v>1</v>
       </c>
       <c r="AG44" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14692,7 +16107,7 @@
         <v>1</v>
       </c>
       <c r="AG45" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14749,7 +16164,7 @@
         <v>1</v>
       </c>
       <c r="AG46" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14806,7 +16221,7 @@
         <v>1</v>
       </c>
       <c r="AG47" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14863,7 +16278,7 @@
         <v>0</v>
       </c>
       <c r="AG48" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14920,7 +16335,7 @@
         <v>1</v>
       </c>
       <c r="AG49" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -14977,7 +16392,7 @@
         <v>1</v>
       </c>
       <c r="AG50" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15034,7 +16449,7 @@
         <v>0</v>
       </c>
       <c r="AG51" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15091,7 +16506,7 @@
         <v>1</v>
       </c>
       <c r="AG52" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15148,7 +16563,7 @@
         <v>1</v>
       </c>
       <c r="AG53" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15205,7 +16620,7 @@
         <v>1</v>
       </c>
       <c r="AG54" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15262,7 +16677,7 @@
         <v>0</v>
       </c>
       <c r="AG55" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15319,7 +16734,7 @@
         <v>1</v>
       </c>
       <c r="AG56" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15376,7 +16791,7 @@
         <v>1</v>
       </c>
       <c r="AG57" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15433,7 +16848,7 @@
         <v>0</v>
       </c>
       <c r="AG58" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15490,7 +16905,7 @@
         <v>1</v>
       </c>
       <c r="AG59" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15547,7 +16962,7 @@
         <v>1</v>
       </c>
       <c r="AG60" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15604,7 +17019,7 @@
         <v>1</v>
       </c>
       <c r="AG61" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15661,7 +17076,7 @@
         <v>1</v>
       </c>
       <c r="AG62" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15718,7 +17133,7 @@
         <v>0</v>
       </c>
       <c r="AG63" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15775,7 +17190,7 @@
         <v>1</v>
       </c>
       <c r="AG64" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15832,7 +17247,7 @@
         <v>1</v>
       </c>
       <c r="AG65" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15889,7 +17304,7 @@
         <v>0</v>
       </c>
       <c r="AG66" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -15946,7 +17361,7 @@
         <v>1</v>
       </c>
       <c r="AG67" t="str">
-        <f t="shared" ref="AG67:AG130" si="29">IF(OR(OR(AND(I67&gt;0.5, M67=1, N67=1), AND(I67&lt;0.5, M67=0, N67=1), AND(I67&gt;0.5, M67=0, N67=0), AND(I67&lt;0.5, M67=1, N67=0)), OR(AND(J67&gt;0.5, M67=1, O67=1), AND(J67&lt;0.5, M67=0, O67=1), AND(J67&gt;0.5, M67=0, O67=0), AND(J67&lt;0.5, M67=1, O67=0)), OR(AND(K67&gt;0.5, M67=1, P67=1), AND(K67&lt;0.5, M67=0, P67=1), AND(K67&gt;0.5, M67=0, P67=0), AND(K67&lt;0.5, M67=1, P67=0)), OR(AND(L67&gt;0.5, M67=1, Q67=1), AND(L67&lt;0.5, M67=0, Q67=1), AND(L67&gt;0.5, M67=0, Q67=0), AND(L67&lt;0.5, M67=1, Q67=0))), "", "XXX")</f>
+        <f t="shared" ref="AG67:AG130" si="30">IF(OR(OR(AND(I67&gt;0.5, M67=1, N67=1), AND(I67&lt;0.5, M67=0, N67=1), AND(I67&gt;0.5, M67=0, N67=0), AND(I67&lt;0.5, M67=1, N67=0)), OR(AND(J67&gt;0.5, M67=1, O67=1), AND(J67&lt;0.5, M67=0, O67=1), AND(J67&gt;0.5, M67=0, O67=0), AND(J67&lt;0.5, M67=1, O67=0)), OR(AND(K67&gt;0.5, M67=1, P67=1), AND(K67&lt;0.5, M67=0, P67=1), AND(K67&gt;0.5, M67=0, P67=0), AND(K67&lt;0.5, M67=1, P67=0)), OR(AND(L67&gt;0.5, M67=1, Q67=1), AND(L67&lt;0.5, M67=0, Q67=1), AND(L67&gt;0.5, M67=0, Q67=0), AND(L67&lt;0.5, M67=1, Q67=0))), "", "XXX")</f>
         <v/>
       </c>
     </row>
@@ -16003,7 +17418,7 @@
         <v>1</v>
       </c>
       <c r="AG68" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16060,7 +17475,7 @@
         <v>0</v>
       </c>
       <c r="AG69" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16117,7 +17532,7 @@
         <v>0</v>
       </c>
       <c r="AG70" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16174,7 +17589,7 @@
         <v>1</v>
       </c>
       <c r="AG71" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16231,7 +17646,7 @@
         <v>1</v>
       </c>
       <c r="AG72" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16288,7 +17703,7 @@
         <v>1</v>
       </c>
       <c r="AG73" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16345,7 +17760,7 @@
         <v>1</v>
       </c>
       <c r="AG74" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16402,7 +17817,7 @@
         <v>0</v>
       </c>
       <c r="AG75" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16459,7 +17874,7 @@
         <v>0</v>
       </c>
       <c r="AG76" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16516,7 +17931,7 @@
         <v>1</v>
       </c>
       <c r="AG77" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16573,7 +17988,7 @@
         <v>1</v>
       </c>
       <c r="AG78" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16630,7 +18045,7 @@
         <v>1</v>
       </c>
       <c r="AG79" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16687,7 +18102,7 @@
         <v>0</v>
       </c>
       <c r="AG80" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16744,7 +18159,7 @@
         <v>1</v>
       </c>
       <c r="AG81" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16801,7 +18216,7 @@
         <v>0</v>
       </c>
       <c r="AG82" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16858,7 +18273,7 @@
         <v>1</v>
       </c>
       <c r="AG83" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16915,7 +18330,7 @@
         <v>1</v>
       </c>
       <c r="AG84" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -16972,7 +18387,7 @@
         <v>0</v>
       </c>
       <c r="AG85" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17029,7 +18444,7 @@
         <v>1</v>
       </c>
       <c r="AG86" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17086,7 +18501,7 @@
         <v>0</v>
       </c>
       <c r="AG87" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17143,7 +18558,7 @@
         <v>1</v>
       </c>
       <c r="AG88" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17200,7 +18615,7 @@
         <v>1</v>
       </c>
       <c r="AG89" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17257,7 +18672,7 @@
         <v>1</v>
       </c>
       <c r="AG90" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17314,7 +18729,7 @@
         <v>1</v>
       </c>
       <c r="AG91" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17371,7 +18786,7 @@
         <v>1</v>
       </c>
       <c r="AG92" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17428,7 +18843,7 @@
         <v>1</v>
       </c>
       <c r="AG93" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17485,7 +18900,7 @@
         <v>1</v>
       </c>
       <c r="AG94" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17542,7 +18957,7 @@
         <v>1</v>
       </c>
       <c r="AG95" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17599,7 +19014,7 @@
         <v>0</v>
       </c>
       <c r="AG96" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17656,7 +19071,7 @@
         <v>1</v>
       </c>
       <c r="AG97" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17713,7 +19128,7 @@
         <v>0</v>
       </c>
       <c r="AG98" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17770,7 +19185,7 @@
         <v>1</v>
       </c>
       <c r="AG99" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17827,7 +19242,7 @@
         <v>0</v>
       </c>
       <c r="AG100" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17884,7 +19299,7 @@
         <v>1</v>
       </c>
       <c r="AG101" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17941,7 +19356,7 @@
         <v>0</v>
       </c>
       <c r="AG102" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -17998,7 +19413,7 @@
         <v>1</v>
       </c>
       <c r="AG103" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18055,7 +19470,7 @@
         <v>0</v>
       </c>
       <c r="AG104" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18112,7 +19527,7 @@
         <v>0</v>
       </c>
       <c r="AG105" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18169,7 +19584,7 @@
         <v>1</v>
       </c>
       <c r="AG106" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18226,7 +19641,7 @@
         <v>1</v>
       </c>
       <c r="AG107" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18283,7 +19698,7 @@
         <v>1</v>
       </c>
       <c r="AG108" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18340,7 +19755,7 @@
         <v>1</v>
       </c>
       <c r="AG109" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18397,7 +19812,7 @@
         <v>0</v>
       </c>
       <c r="AG110" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18454,7 +19869,7 @@
         <v>1</v>
       </c>
       <c r="AG111" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18511,7 +19926,7 @@
         <v>1</v>
       </c>
       <c r="AG112" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18568,7 +19983,7 @@
         <v>1</v>
       </c>
       <c r="AG113" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18625,7 +20040,7 @@
         <v>1</v>
       </c>
       <c r="AG114" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18682,7 +20097,7 @@
         <v>0</v>
       </c>
       <c r="AG115" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18739,7 +20154,7 @@
         <v>1</v>
       </c>
       <c r="AG116" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18796,7 +20211,7 @@
         <v>0</v>
       </c>
       <c r="AG117" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18853,7 +20268,7 @@
         <v>0</v>
       </c>
       <c r="AG118" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18910,7 +20325,7 @@
         <v>1</v>
       </c>
       <c r="AG119" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -18967,7 +20382,7 @@
         <v>0</v>
       </c>
       <c r="AG120" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -19024,7 +20439,7 @@
         <v>1</v>
       </c>
       <c r="AG121" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -19081,7 +20496,7 @@
         <v>1</v>
       </c>
       <c r="AG122" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -19138,7 +20553,7 @@
         <v>1</v>
       </c>
       <c r="AG123" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -19195,7 +20610,7 @@
         <v>0</v>
       </c>
       <c r="AG124" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -19252,7 +20667,7 @@
         <v>1</v>
       </c>
       <c r="AG125" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -19309,7 +20724,7 @@
         <v>1</v>
       </c>
       <c r="AG126" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -19366,7 +20781,7 @@
         <v>1</v>
       </c>
       <c r="AG127" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -19423,7 +20838,7 @@
         <v>1</v>
       </c>
       <c r="AG128" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -19480,7 +20895,7 @@
         <v>1</v>
       </c>
       <c r="AG129" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -19537,7 +20952,7 @@
         <v>1</v>
       </c>
       <c r="AG130" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v/>
       </c>
     </row>
@@ -19594,7 +21009,7 @@
         <v>0</v>
       </c>
       <c r="AG131" t="str">
-        <f t="shared" ref="AG131:AG194" si="30">IF(OR(OR(AND(I131&gt;0.5, M131=1, N131=1), AND(I131&lt;0.5, M131=0, N131=1), AND(I131&gt;0.5, M131=0, N131=0), AND(I131&lt;0.5, M131=1, N131=0)), OR(AND(J131&gt;0.5, M131=1, O131=1), AND(J131&lt;0.5, M131=0, O131=1), AND(J131&gt;0.5, M131=0, O131=0), AND(J131&lt;0.5, M131=1, O131=0)), OR(AND(K131&gt;0.5, M131=1, P131=1), AND(K131&lt;0.5, M131=0, P131=1), AND(K131&gt;0.5, M131=0, P131=0), AND(K131&lt;0.5, M131=1, P131=0)), OR(AND(L131&gt;0.5, M131=1, Q131=1), AND(L131&lt;0.5, M131=0, Q131=1), AND(L131&gt;0.5, M131=0, Q131=0), AND(L131&lt;0.5, M131=1, Q131=0))), "", "XXX")</f>
+        <f t="shared" ref="AG131:AG194" si="31">IF(OR(OR(AND(I131&gt;0.5, M131=1, N131=1), AND(I131&lt;0.5, M131=0, N131=1), AND(I131&gt;0.5, M131=0, N131=0), AND(I131&lt;0.5, M131=1, N131=0)), OR(AND(J131&gt;0.5, M131=1, O131=1), AND(J131&lt;0.5, M131=0, O131=1), AND(J131&gt;0.5, M131=0, O131=0), AND(J131&lt;0.5, M131=1, O131=0)), OR(AND(K131&gt;0.5, M131=1, P131=1), AND(K131&lt;0.5, M131=0, P131=1), AND(K131&gt;0.5, M131=0, P131=0), AND(K131&lt;0.5, M131=1, P131=0)), OR(AND(L131&gt;0.5, M131=1, Q131=1), AND(L131&lt;0.5, M131=0, Q131=1), AND(L131&gt;0.5, M131=0, Q131=0), AND(L131&lt;0.5, M131=1, Q131=0))), "", "XXX")</f>
         <v/>
       </c>
     </row>
@@ -19651,7 +21066,7 @@
         <v>0</v>
       </c>
       <c r="AG132" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -19708,7 +21123,7 @@
         <v>0</v>
       </c>
       <c r="AG133" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -19765,7 +21180,7 @@
         <v>1</v>
       </c>
       <c r="AG134" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -19822,7 +21237,7 @@
         <v>0</v>
       </c>
       <c r="AG135" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -19879,7 +21294,7 @@
         <v>1</v>
       </c>
       <c r="AG136" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -19936,7 +21351,7 @@
         <v>1</v>
       </c>
       <c r="AG137" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -19993,7 +21408,7 @@
         <v>1</v>
       </c>
       <c r="AG138" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20050,7 +21465,7 @@
         <v>0</v>
       </c>
       <c r="AG139" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20107,7 +21522,7 @@
         <v>1</v>
       </c>
       <c r="AG140" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20164,7 +21579,7 @@
         <v>1</v>
       </c>
       <c r="AG141" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20221,7 +21636,7 @@
         <v>1</v>
       </c>
       <c r="AG142" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20278,7 +21693,7 @@
         <v>0</v>
       </c>
       <c r="AG143" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20335,7 +21750,7 @@
         <v>0</v>
       </c>
       <c r="AG144" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20392,7 +21807,7 @@
         <v>0</v>
       </c>
       <c r="AG145" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20449,7 +21864,7 @@
         <v>1</v>
       </c>
       <c r="AG146" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20506,7 +21921,7 @@
         <v>1</v>
       </c>
       <c r="AG147" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20563,7 +21978,7 @@
         <v>0</v>
       </c>
       <c r="AG148" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20620,7 +22035,7 @@
         <v>0</v>
       </c>
       <c r="AG149" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20677,7 +22092,7 @@
         <v>1</v>
       </c>
       <c r="AG150" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20734,7 +22149,7 @@
         <v>0</v>
       </c>
       <c r="AG151" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20791,7 +22206,7 @@
         <v>1</v>
       </c>
       <c r="AG152" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20848,7 +22263,7 @@
         <v>1</v>
       </c>
       <c r="AG153" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20905,7 +22320,7 @@
         <v>0</v>
       </c>
       <c r="AG154" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -20962,7 +22377,7 @@
         <v>1</v>
       </c>
       <c r="AG155" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21019,7 +22434,7 @@
         <v>1</v>
       </c>
       <c r="AG156" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21076,7 +22491,7 @@
         <v>1</v>
       </c>
       <c r="AG157" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21133,7 +22548,7 @@
         <v>1</v>
       </c>
       <c r="AG158" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21190,7 +22605,7 @@
         <v>0</v>
       </c>
       <c r="AG159" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21247,7 +22662,7 @@
         <v>0</v>
       </c>
       <c r="AG160" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21304,7 +22719,7 @@
         <v>1</v>
       </c>
       <c r="AG161" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21361,7 +22776,7 @@
         <v>1</v>
       </c>
       <c r="AG162" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21418,7 +22833,7 @@
         <v>1</v>
       </c>
       <c r="AG163" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21475,7 +22890,7 @@
         <v>1</v>
       </c>
       <c r="AG164" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21532,7 +22947,7 @@
         <v>1</v>
       </c>
       <c r="AG165" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21589,7 +23004,7 @@
         <v>1</v>
       </c>
       <c r="AG166" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21646,7 +23061,7 @@
         <v>1</v>
       </c>
       <c r="AG167" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21703,7 +23118,7 @@
         <v>0</v>
       </c>
       <c r="AG168" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21760,7 +23175,7 @@
         <v>0</v>
       </c>
       <c r="AG169" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21817,7 +23232,7 @@
         <v>1</v>
       </c>
       <c r="AG170" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21874,7 +23289,7 @@
         <v>1</v>
       </c>
       <c r="AG171" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21931,7 +23346,7 @@
         <v>1</v>
       </c>
       <c r="AG172" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -21988,7 +23403,7 @@
         <v>1</v>
       </c>
       <c r="AG173" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22045,7 +23460,7 @@
         <v>1</v>
       </c>
       <c r="AG174" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22102,7 +23517,7 @@
         <v>0</v>
       </c>
       <c r="AG175" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22159,7 +23574,7 @@
         <v>1</v>
       </c>
       <c r="AG176" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22216,7 +23631,7 @@
         <v>1</v>
       </c>
       <c r="AG177" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22273,7 +23688,7 @@
         <v>0</v>
       </c>
       <c r="AG178" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22330,7 +23745,7 @@
         <v>0</v>
       </c>
       <c r="AG179" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22387,7 +23802,7 @@
         <v>1</v>
       </c>
       <c r="AG180" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22444,7 +23859,7 @@
         <v>1</v>
       </c>
       <c r="AG181" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22501,7 +23916,7 @@
         <v>0</v>
       </c>
       <c r="AG182" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22558,7 +23973,7 @@
         <v>1</v>
       </c>
       <c r="AG183" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22615,7 +24030,7 @@
         <v>0</v>
       </c>
       <c r="AG184" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22672,7 +24087,7 @@
         <v>1</v>
       </c>
       <c r="AG185" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22729,7 +24144,7 @@
         <v>0</v>
       </c>
       <c r="AG186" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22786,7 +24201,7 @@
         <v>0</v>
       </c>
       <c r="AG187" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22843,7 +24258,7 @@
         <v>0</v>
       </c>
       <c r="AG188" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22900,7 +24315,7 @@
         <v>1</v>
       </c>
       <c r="AG189" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -22957,7 +24372,7 @@
         <v>1</v>
       </c>
       <c r="AG190" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -23014,7 +24429,7 @@
         <v>1</v>
       </c>
       <c r="AG191" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -23071,7 +24486,7 @@
         <v>1</v>
       </c>
       <c r="AG192" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -23128,7 +24543,7 @@
         <v>1</v>
       </c>
       <c r="AG193" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -23185,7 +24600,7 @@
         <v>1</v>
       </c>
       <c r="AG194" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v/>
       </c>
     </row>
@@ -23242,7 +24657,7 @@
         <v>0</v>
       </c>
       <c r="AG195" t="str">
-        <f t="shared" ref="AG195:AG257" si="31">IF(OR(OR(AND(I195&gt;0.5, M195=1, N195=1), AND(I195&lt;0.5, M195=0, N195=1), AND(I195&gt;0.5, M195=0, N195=0), AND(I195&lt;0.5, M195=1, N195=0)), OR(AND(J195&gt;0.5, M195=1, O195=1), AND(J195&lt;0.5, M195=0, O195=1), AND(J195&gt;0.5, M195=0, O195=0), AND(J195&lt;0.5, M195=1, O195=0)), OR(AND(K195&gt;0.5, M195=1, P195=1), AND(K195&lt;0.5, M195=0, P195=1), AND(K195&gt;0.5, M195=0, P195=0), AND(K195&lt;0.5, M195=1, P195=0)), OR(AND(L195&gt;0.5, M195=1, Q195=1), AND(L195&lt;0.5, M195=0, Q195=1), AND(L195&gt;0.5, M195=0, Q195=0), AND(L195&lt;0.5, M195=1, Q195=0))), "", "XXX")</f>
+        <f t="shared" ref="AG195:AG257" si="32">IF(OR(OR(AND(I195&gt;0.5, M195=1, N195=1), AND(I195&lt;0.5, M195=0, N195=1), AND(I195&gt;0.5, M195=0, N195=0), AND(I195&lt;0.5, M195=1, N195=0)), OR(AND(J195&gt;0.5, M195=1, O195=1), AND(J195&lt;0.5, M195=0, O195=1), AND(J195&gt;0.5, M195=0, O195=0), AND(J195&lt;0.5, M195=1, O195=0)), OR(AND(K195&gt;0.5, M195=1, P195=1), AND(K195&lt;0.5, M195=0, P195=1), AND(K195&gt;0.5, M195=0, P195=0), AND(K195&lt;0.5, M195=1, P195=0)), OR(AND(L195&gt;0.5, M195=1, Q195=1), AND(L195&lt;0.5, M195=0, Q195=1), AND(L195&gt;0.5, M195=0, Q195=0), AND(L195&lt;0.5, M195=1, Q195=0))), "", "XXX")</f>
         <v/>
       </c>
     </row>
@@ -23299,7 +24714,7 @@
         <v>0</v>
       </c>
       <c r="AG196" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -23356,7 +24771,7 @@
         <v>0</v>
       </c>
       <c r="AG197" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -23413,7 +24828,7 @@
         <v>1</v>
       </c>
       <c r="AG198" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -23470,7 +24885,7 @@
         <v>0</v>
       </c>
       <c r="AG199" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -23527,7 +24942,7 @@
         <v>1</v>
       </c>
       <c r="AG200" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -23584,7 +24999,7 @@
         <v>0</v>
       </c>
       <c r="AG201" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -23641,7 +25056,7 @@
         <v>1</v>
       </c>
       <c r="AG202" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -23698,7 +25113,7 @@
         <v>0</v>
       </c>
       <c r="AG203" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -23755,7 +25170,7 @@
         <v>1</v>
       </c>
       <c r="AG204" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -23812,7 +25227,7 @@
         <v>0</v>
       </c>
       <c r="AG205" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -23869,7 +25284,7 @@
         <v>1</v>
       </c>
       <c r="AG206" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -23926,7 +25341,7 @@
         <v>1</v>
       </c>
       <c r="AG207" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -23983,7 +25398,7 @@
         <v>0</v>
       </c>
       <c r="AG208" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24040,7 +25455,7 @@
         <v>1</v>
       </c>
       <c r="AG209" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24097,7 +25512,7 @@
         <v>0</v>
       </c>
       <c r="AG210" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24154,7 +25569,7 @@
         <v>0</v>
       </c>
       <c r="AG211" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24211,7 +25626,7 @@
         <v>1</v>
       </c>
       <c r="AG212" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24268,7 +25683,7 @@
         <v>1</v>
       </c>
       <c r="AG213" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24325,7 +25740,7 @@
         <v>1</v>
       </c>
       <c r="AG214" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24382,7 +25797,7 @@
         <v>1</v>
       </c>
       <c r="AG215" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24439,7 +25854,7 @@
         <v>1</v>
       </c>
       <c r="AG216" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24496,7 +25911,7 @@
         <v>1</v>
       </c>
       <c r="AG217" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24553,7 +25968,7 @@
         <v>1</v>
       </c>
       <c r="AG218" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24610,7 +26025,7 @@
         <v>0</v>
       </c>
       <c r="AG219" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24667,7 +26082,7 @@
         <v>1</v>
       </c>
       <c r="AG220" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24724,7 +26139,7 @@
         <v>0</v>
       </c>
       <c r="AG221" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24781,7 +26196,7 @@
         <v>0</v>
       </c>
       <c r="AG222" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24838,7 +26253,7 @@
         <v>1</v>
       </c>
       <c r="AG223" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24895,7 +26310,7 @@
         <v>0</v>
       </c>
       <c r="AG224" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -24952,7 +26367,7 @@
         <v>1</v>
       </c>
       <c r="AG225" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25009,7 +26424,7 @@
         <v>1</v>
       </c>
       <c r="AG226" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25066,7 +26481,7 @@
         <v>0</v>
       </c>
       <c r="AG227" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25123,7 +26538,7 @@
         <v>0</v>
       </c>
       <c r="AG228" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25180,7 +26595,7 @@
         <v>1</v>
       </c>
       <c r="AG229" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25237,7 +26652,7 @@
         <v>1</v>
       </c>
       <c r="AG230" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25294,7 +26709,7 @@
         <v>1</v>
       </c>
       <c r="AG231" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25351,7 +26766,7 @@
         <v>1</v>
       </c>
       <c r="AG232" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25408,7 +26823,7 @@
         <v>0</v>
       </c>
       <c r="AG233" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25465,7 +26880,7 @@
         <v>1</v>
       </c>
       <c r="AG234" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25522,7 +26937,7 @@
         <v>1</v>
       </c>
       <c r="AG235" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25579,7 +26994,7 @@
         <v>1</v>
       </c>
       <c r="AG236" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25636,7 +27051,7 @@
         <v>1</v>
       </c>
       <c r="AG237" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25693,7 +27108,7 @@
         <v>1</v>
       </c>
       <c r="AG238" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25750,7 +27165,7 @@
         <v>1</v>
       </c>
       <c r="AG239" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25807,7 +27222,7 @@
         <v>0</v>
       </c>
       <c r="AG240" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25864,7 +27279,7 @@
         <v>0</v>
       </c>
       <c r="AG241" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25921,7 +27336,7 @@
         <v>1</v>
       </c>
       <c r="AG242" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -25978,7 +27393,7 @@
         <v>1</v>
       </c>
       <c r="AG243" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26035,7 +27450,7 @@
         <v>0</v>
       </c>
       <c r="AG244" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26092,7 +27507,7 @@
         <v>1</v>
       </c>
       <c r="AG245" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26149,7 +27564,7 @@
         <v>1</v>
       </c>
       <c r="AG246" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26206,7 +27621,7 @@
         <v>0</v>
       </c>
       <c r="AG247" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26263,7 +27678,7 @@
         <v>1</v>
       </c>
       <c r="AG248" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26320,7 +27735,7 @@
         <v>0</v>
       </c>
       <c r="AG249" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26377,7 +27792,7 @@
         <v>0</v>
       </c>
       <c r="AG250" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26434,7 +27849,7 @@
         <v>1</v>
       </c>
       <c r="AG251" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26491,7 +27906,7 @@
         <v>1</v>
       </c>
       <c r="AG252" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26548,7 +27963,7 @@
         <v>1</v>
       </c>
       <c r="AG253" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26605,7 +28020,7 @@
         <v>1</v>
       </c>
       <c r="AG254" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26662,7 +28077,7 @@
         <v>1</v>
       </c>
       <c r="AG255" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26719,7 +28134,7 @@
         <v>1</v>
       </c>
       <c r="AG256" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26776,7 +28191,7 @@
         <v>1</v>
       </c>
       <c r="AG257" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v/>
       </c>
     </row>
@@ -26809,8 +28224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E0EE4BA-B59F-4CB3-B656-48863F2CA16F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M103" sqref="M103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>